<commit_message>
Update help and example sheet links.
</commit_message>
<xml_diff>
--- a/ExcelExamples/BermudanSwaption.xlsx
+++ b/ExcelExamples/BermudanSwaption.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="75" windowWidth="18195" windowHeight="10290" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="72" windowWidth="18192" windowHeight="10296"/>
   </bookViews>
   <sheets>
     <sheet name="Varying exercise dates" sheetId="3" r:id="rId1"/>
     <sheet name="Product&amp;EPE" sheetId="2" r:id="rId2"/>
     <sheet name="Model" sheetId="1" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621" calcMode="manual" calcOnSave="0"/>
+  <calcPr calcId="145621" calcMode="manual" calcCompleted="0" calcOnSave="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="36">
   <si>
     <t>name</t>
   </si>
@@ -118,6 +118,12 @@
   </si>
   <si>
     <t>Swaption4Ex</t>
+  </si>
+  <si>
+    <t>QSA.GetAvailableResults</t>
+  </si>
+  <si>
+    <t>QSA.GetResults</t>
   </si>
 </sst>
 </file>
@@ -1036,11 +1042,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="373040256"/>
-        <c:axId val="373045504"/>
+        <c:axId val="265243264"/>
+        <c:axId val="265253248"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="373040256"/>
+        <c:axId val="265243264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1050,14 +1056,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="373045504"/>
+        <c:crossAx val="265253248"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="373045504"/>
+        <c:axId val="265253248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1068,7 +1074,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="373040256"/>
+        <c:crossAx val="265243264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1409,31 +1415,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:E24"/>
+  <dimension ref="B2:E27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C21" sqref="C21:C24"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="44.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="33.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="44.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:5" ht="15" x14ac:dyDescent="0.25">
       <c r="E2" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:5" ht="15" x14ac:dyDescent="0.25">
       <c r="E3" s="7">
         <v>43040</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:5" ht="15" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>28</v>
       </c>
@@ -1444,7 +1450,7 @@
         <v>43405</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:5" ht="15" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>13</v>
       </c>
@@ -1455,7 +1461,7 @@
         <v>43770</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:5" ht="15" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>14</v>
       </c>
@@ -1466,7 +1472,7 @@
         <v>44136</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:5" ht="15" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>16</v>
       </c>
@@ -1474,7 +1480,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:5" ht="15" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
         <v>17</v>
       </c>
@@ -1482,7 +1488,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:5" ht="15" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
         <v>18</v>
       </c>
@@ -1495,7 +1501,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:5" ht="15" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
         <v>0</v>
       </c>
@@ -1507,7 +1513,7 @@
         <v>Swaption1Ex.09:10:26-122</v>
       </c>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:5" ht="15" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
         <v>0</v>
       </c>
@@ -1519,7 +1525,7 @@
         <v>Swaption2Ex.09:10:26-119</v>
       </c>
     </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:5" ht="15" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
         <v>0</v>
       </c>
@@ -1531,7 +1537,7 @@
         <v>Swaption3Ex.09:10:26-120</v>
       </c>
     </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:5" ht="15" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
         <v>0</v>
       </c>
@@ -1543,7 +1549,7 @@
         <v>Swaption4Ex.09:10:26-121</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B17" s="2" t="s">
         <v>21</v>
       </c>
@@ -1552,7 +1558,7 @@
         <v>42675</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B18" s="2" t="s">
         <v>23</v>
       </c>
@@ -1561,7 +1567,7 @@
         <v>HWDemo.09:10:26-124</v>
       </c>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B19" s="2" t="s">
         <v>24</v>
       </c>
@@ -1569,43 +1575,59 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B21" s="3" t="str">
+    <row r="21" spans="2:3" ht="21" x14ac:dyDescent="0.4">
+      <c r="C21" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" ht="21" x14ac:dyDescent="0.4">
+      <c r="C22" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="C23" t="str">
+        <f ca="1">_xll.QSA.GetAvailableResults(B24)</f>
+        <v>value</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B24" s="3" t="str">
         <f>_xll.QSA.Value(C12&amp;"Value",D12,$C$17,$C$18,$C$19)</f>
         <v>Swaption1ExValue.09:10:26-125</v>
       </c>
-      <c r="C21" s="11">
-        <f>_xll.QSA.GetResults(B21,"value")</f>
+      <c r="C24" s="11">
+        <f>_xll.QSA.GetResults(B24,"value")</f>
         <v>-9597.2890686645351</v>
       </c>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B22" s="3" t="str">
+    <row r="25" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B25" s="3" t="str">
         <f>_xll.QSA.Value(C13&amp;"Value",D13,$C$17,$C$18,$C$19)</f>
         <v>Swaption2ExValue.09:10:28-128</v>
       </c>
-      <c r="C22" s="11">
-        <f>_xll.QSA.GetResults(B22,"value")</f>
+      <c r="C25" s="11">
+        <f>_xll.QSA.GetResults(B25,"value")</f>
         <v>-11978.432212997121</v>
       </c>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B23" s="3" t="str">
+    <row r="26" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B26" s="3" t="str">
         <f>_xll.QSA.Value(C14&amp;"Value",D14,$C$17,$C$18,$C$19)</f>
         <v>Swaption3ExValue.09:10:27-127</v>
       </c>
-      <c r="C23" s="11">
-        <f>_xll.QSA.GetResults(B23,"value")</f>
+      <c r="C26" s="11">
+        <f>_xll.QSA.GetResults(B26,"value")</f>
         <v>-12965.151497549465</v>
       </c>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B24" s="3" t="str">
+    <row r="27" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B27" s="3" t="str">
         <f>_xll.QSA.Value(C15&amp;"Value",D15,$C$17,$C$18,$C$19)</f>
         <v>Swaption4ExValue.09:10:27-126</v>
       </c>
-      <c r="C24" s="11">
-        <f>_xll.QSA.GetResults(B24,"value")</f>
+      <c r="C27" s="11">
+        <f>_xll.QSA.GetResults(B27,"value")</f>
         <v>-13296.063937555664</v>
       </c>
     </row>
@@ -1618,18 +1640,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E146"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F64" sqref="F64"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="27.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="33.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:5" ht="15" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1640,12 +1662,12 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:5" ht="15" x14ac:dyDescent="0.25">
       <c r="E3" s="7">
         <v>43040</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:5" ht="15" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>28</v>
       </c>
@@ -1656,7 +1678,7 @@
         <v>43405</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:5" ht="15" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>13</v>
       </c>
@@ -1667,7 +1689,7 @@
         <v>43770</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:5" ht="15" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>14</v>
       </c>
@@ -1678,7 +1700,7 @@
         <v>44136</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:5" ht="15" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>16</v>
       </c>
@@ -1686,7 +1708,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:5" ht="15" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
         <v>17</v>
       </c>
@@ -1694,7 +1716,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:5" ht="15" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
         <v>18</v>
       </c>
@@ -1707,13 +1729,13 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:5" ht="15" x14ac:dyDescent="0.25">
       <c r="B12" s="3" t="str">
         <f>_xll.QSA.CreateZARBermudanSwaption(C2,E3:E4,C4,C5,C6,C7,C8,C9)</f>
         <v>BermudanSwaption0001.09:10:26-118</v>
       </c>
     </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:5" ht="15" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
         <v>0</v>
       </c>
@@ -1721,7 +1743,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:5" ht="15" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="s">
         <v>19</v>
       </c>
@@ -1730,7 +1752,7 @@
         <v>BermudanSwaption0001.09:10:26-118</v>
       </c>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B19" s="2" t="s">
         <v>21</v>
       </c>
@@ -1739,7 +1761,7 @@
         <v>42675</v>
       </c>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B20" s="2" t="s">
         <v>23</v>
       </c>
@@ -1748,7 +1770,7 @@
         <v>HWDemo.09:10:26-124</v>
       </c>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B21" s="2" t="s">
         <v>24</v>
       </c>
@@ -1761,12 +1783,12 @@
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B24" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B25" s="7">
         <f>C19</f>
         <v>42675</v>
@@ -1776,7 +1798,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B26" s="7">
         <f>B25+15</f>
         <v>42690</v>
@@ -1785,7 +1807,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B27" s="7">
         <f t="shared" ref="B27:B90" si="0">B26+15</f>
         <v>42705</v>
@@ -1794,7 +1816,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B28" s="7">
         <f t="shared" si="0"/>
         <v>42720</v>
@@ -1803,7 +1825,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B29" s="7">
         <f t="shared" si="0"/>
         <v>42735</v>
@@ -1812,7 +1834,7 @@
         <v>0.58766449057314163</v>
       </c>
     </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B30" s="7">
         <f t="shared" si="0"/>
         <v>42750</v>
@@ -1821,7 +1843,7 @@
         <v>0.33330954272205415</v>
       </c>
     </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B31" s="7">
         <f t="shared" si="0"/>
         <v>42765</v>
@@ -1830,7 +1852,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B32" s="7">
         <f t="shared" si="0"/>
         <v>42780</v>
@@ -1839,7 +1861,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B33" s="7">
         <f t="shared" si="0"/>
         <v>42795</v>
@@ -1848,7 +1870,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B34" s="7">
         <f t="shared" si="0"/>
         <v>42810</v>
@@ -1857,7 +1879,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B35" s="7">
         <f t="shared" si="0"/>
         <v>42825</v>
@@ -1866,7 +1888,7 @@
         <v>0.16095383044728206</v>
       </c>
     </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B36" s="7">
         <f t="shared" si="0"/>
         <v>42840</v>
@@ -1875,7 +1897,7 @@
         <v>2.287870045080393</v>
       </c>
     </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B37" s="7">
         <f t="shared" si="0"/>
         <v>42855</v>
@@ -1884,7 +1906,7 @@
         <v>0.45330458066640766</v>
       </c>
     </row>
-    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B38" s="7">
         <f t="shared" si="0"/>
         <v>42870</v>
@@ -1893,7 +1915,7 @@
         <v>2.4650942759317331</v>
       </c>
     </row>
-    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B39" s="7">
         <f t="shared" si="0"/>
         <v>42885</v>
@@ -1902,7 +1924,7 @@
         <v>0.3435804514881779</v>
       </c>
     </row>
-    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B40" s="7">
         <f t="shared" si="0"/>
         <v>42900</v>
@@ -1911,7 +1933,7 @@
         <v>6.4394953071166761</v>
       </c>
     </row>
-    <row r="41" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B41" s="7">
         <f t="shared" si="0"/>
         <v>42915</v>
@@ -1920,7 +1942,7 @@
         <v>15.432070455697964</v>
       </c>
     </row>
-    <row r="42" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B42" s="7">
         <f t="shared" si="0"/>
         <v>42930</v>
@@ -1929,7 +1951,7 @@
         <v>12.606054757416631</v>
       </c>
     </row>
-    <row r="43" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B43" s="7">
         <f t="shared" si="0"/>
         <v>42945</v>
@@ -1938,7 +1960,7 @@
         <v>12.457713634014713</v>
       </c>
     </row>
-    <row r="44" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B44" s="7">
         <f t="shared" si="0"/>
         <v>42960</v>
@@ -1947,7 +1969,7 @@
         <v>10.686992351896832</v>
       </c>
     </row>
-    <row r="45" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B45" s="7">
         <f t="shared" si="0"/>
         <v>42975</v>
@@ -1956,7 +1978,7 @@
         <v>12.195249894161828</v>
       </c>
     </row>
-    <row r="46" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B46" s="7">
         <f t="shared" si="0"/>
         <v>42990</v>
@@ -1965,7 +1987,7 @@
         <v>11.294221892745716</v>
       </c>
     </row>
-    <row r="47" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B47" s="7">
         <f t="shared" si="0"/>
         <v>43005</v>
@@ -1974,7 +1996,7 @@
         <v>9.4098841146912946</v>
       </c>
     </row>
-    <row r="48" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B48" s="7">
         <f t="shared" si="0"/>
         <v>43020</v>
@@ -1983,7 +2005,7 @@
         <v>3.7370042565768635</v>
       </c>
     </row>
-    <row r="49" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B49" s="7">
         <f t="shared" si="0"/>
         <v>43035</v>
@@ -1992,7 +2014,7 @@
         <v>3.884872441489903</v>
       </c>
     </row>
-    <row r="50" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B50" s="7">
         <f t="shared" si="0"/>
         <v>43050</v>
@@ -2001,7 +2023,7 @@
         <v>6.6806074316484079</v>
       </c>
     </row>
-    <row r="51" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B51" s="7">
         <f t="shared" si="0"/>
         <v>43065</v>
@@ -2010,7 +2032,7 @@
         <v>5.2818599662227257</v>
       </c>
     </row>
-    <row r="52" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B52" s="7">
         <f t="shared" si="0"/>
         <v>43080</v>
@@ -2019,7 +2041,7 @@
         <v>5.0306173714740856</v>
       </c>
     </row>
-    <row r="53" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B53" s="7">
         <f t="shared" si="0"/>
         <v>43095</v>
@@ -2028,7 +2050,7 @@
         <v>5.0769801450758747</v>
       </c>
     </row>
-    <row r="54" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B54" s="7">
         <f t="shared" si="0"/>
         <v>43110</v>
@@ -2037,7 +2059,7 @@
         <v>5.5724967934043761</v>
       </c>
     </row>
-    <row r="55" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B55" s="7">
         <f t="shared" si="0"/>
         <v>43125</v>
@@ -2046,7 +2068,7 @@
         <v>4.1951096947929578</v>
       </c>
     </row>
-    <row r="56" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B56" s="7">
         <f t="shared" si="0"/>
         <v>43140</v>
@@ -2055,7 +2077,7 @@
         <v>2.3875447715824505</v>
       </c>
     </row>
-    <row r="57" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B57" s="7">
         <f t="shared" si="0"/>
         <v>43155</v>
@@ -2064,7 +2086,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B58" s="7">
         <f t="shared" si="0"/>
         <v>43170</v>
@@ -2073,7 +2095,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B59" s="7">
         <f t="shared" si="0"/>
         <v>43185</v>
@@ -2082,7 +2104,7 @@
         <v>0.91050756464516125</v>
       </c>
     </row>
-    <row r="60" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B60" s="7">
         <f t="shared" si="0"/>
         <v>43200</v>
@@ -2091,7 +2113,7 @@
         <v>14.207884605877252</v>
       </c>
     </row>
-    <row r="61" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B61" s="7">
         <f t="shared" si="0"/>
         <v>43215</v>
@@ -2100,7 +2122,7 @@
         <v>20.08437522096602</v>
       </c>
     </row>
-    <row r="62" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B62" s="7">
         <f t="shared" si="0"/>
         <v>43230</v>
@@ -2109,7 +2131,7 @@
         <v>37.248532479395813</v>
       </c>
     </row>
-    <row r="63" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B63" s="7">
         <f t="shared" si="0"/>
         <v>43245</v>
@@ -2118,7 +2140,7 @@
         <v>93.48921668815882</v>
       </c>
     </row>
-    <row r="64" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B64" s="7">
         <f t="shared" si="0"/>
         <v>43260</v>
@@ -2127,7 +2149,7 @@
         <v>140.07363864430579</v>
       </c>
     </row>
-    <row r="65" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B65" s="7">
         <f t="shared" si="0"/>
         <v>43275</v>
@@ -2136,7 +2158,7 @@
         <v>219.48755143385762</v>
       </c>
     </row>
-    <row r="66" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B66" s="7">
         <f t="shared" si="0"/>
         <v>43290</v>
@@ -2145,7 +2167,7 @@
         <v>257.50144333128566</v>
       </c>
     </row>
-    <row r="67" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B67" s="7">
         <f t="shared" si="0"/>
         <v>43305</v>
@@ -2154,7 +2176,7 @@
         <v>287.58051598618971</v>
       </c>
     </row>
-    <row r="68" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B68" s="7">
         <f t="shared" si="0"/>
         <v>43320</v>
@@ -2163,7 +2185,7 @@
         <v>345.71963364839581</v>
       </c>
     </row>
-    <row r="69" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B69" s="7">
         <f t="shared" si="0"/>
         <v>43335</v>
@@ -2172,7 +2194,7 @@
         <v>418.9177123749684</v>
       </c>
     </row>
-    <row r="70" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B70" s="7">
         <f t="shared" si="0"/>
         <v>43350</v>
@@ -2181,7 +2203,7 @@
         <v>484.14215321555065</v>
       </c>
     </row>
-    <row r="71" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B71" s="7">
         <f t="shared" si="0"/>
         <v>43365</v>
@@ -2190,7 +2212,7 @@
         <v>534.1174176641432</v>
       </c>
     </row>
-    <row r="72" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B72" s="7">
         <f t="shared" si="0"/>
         <v>43380</v>
@@ -2199,7 +2221,7 @@
         <v>596.81580883009633</v>
       </c>
     </row>
-    <row r="73" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B73" s="7">
         <f t="shared" si="0"/>
         <v>43395</v>
@@ -2208,7 +2230,7 @@
         <v>641.85927527087085</v>
       </c>
     </row>
-    <row r="74" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B74" s="7">
         <f t="shared" si="0"/>
         <v>43410</v>
@@ -2217,7 +2239,7 @@
         <v>646.78994567192058</v>
       </c>
     </row>
-    <row r="75" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B75" s="7">
         <f t="shared" si="0"/>
         <v>43425</v>
@@ -2226,7 +2248,7 @@
         <v>677.83475841021925</v>
       </c>
     </row>
-    <row r="76" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B76" s="7">
         <f t="shared" si="0"/>
         <v>43440</v>
@@ -2235,7 +2257,7 @@
         <v>711.35828379384827</v>
       </c>
     </row>
-    <row r="77" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B77" s="7">
         <f t="shared" si="0"/>
         <v>43455</v>
@@ -2244,7 +2266,7 @@
         <v>776.4477956452115</v>
       </c>
     </row>
-    <row r="78" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B78" s="7">
         <f t="shared" si="0"/>
         <v>43470</v>
@@ -2253,7 +2275,7 @@
         <v>837.04067831908981</v>
       </c>
     </row>
-    <row r="79" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B79" s="7">
         <f t="shared" si="0"/>
         <v>43485</v>
@@ -2262,7 +2284,7 @@
         <v>903.93467461764351</v>
       </c>
     </row>
-    <row r="80" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B80" s="7">
         <f t="shared" si="0"/>
         <v>43500</v>
@@ -2271,7 +2293,7 @@
         <v>946.65568584893754</v>
       </c>
     </row>
-    <row r="81" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B81" s="7">
         <f t="shared" si="0"/>
         <v>43515</v>
@@ -2280,7 +2302,7 @@
         <v>1012.7239831227166</v>
       </c>
     </row>
-    <row r="82" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B82" s="7">
         <f t="shared" si="0"/>
         <v>43530</v>
@@ -2289,7 +2311,7 @@
         <v>1017.3593473935928</v>
       </c>
     </row>
-    <row r="83" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B83" s="7">
         <f t="shared" si="0"/>
         <v>43545</v>
@@ -2298,7 +2320,7 @@
         <v>1087.4820314195929</v>
       </c>
     </row>
-    <row r="84" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B84" s="7">
         <f t="shared" si="0"/>
         <v>43560</v>
@@ -2307,7 +2329,7 @@
         <v>1160.9007706132393</v>
       </c>
     </row>
-    <row r="85" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B85" s="7">
         <f t="shared" si="0"/>
         <v>43575</v>
@@ -2316,7 +2338,7 @@
         <v>1236.2772736675643</v>
       </c>
     </row>
-    <row r="86" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B86" s="7">
         <f t="shared" si="0"/>
         <v>43590</v>
@@ -2325,7 +2347,7 @@
         <v>1243.7606195230567</v>
       </c>
     </row>
-    <row r="87" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B87" s="7">
         <f t="shared" si="0"/>
         <v>43605</v>
@@ -2334,7 +2356,7 @@
         <v>1292.5399230650826</v>
       </c>
     </row>
-    <row r="88" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B88" s="7">
         <f t="shared" si="0"/>
         <v>43620</v>
@@ -2343,7 +2365,7 @@
         <v>1361.4491862225104</v>
       </c>
     </row>
-    <row r="89" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B89" s="7">
         <f t="shared" si="0"/>
         <v>43635</v>
@@ -2352,7 +2374,7 @@
         <v>1414.2334161517551</v>
       </c>
     </row>
-    <row r="90" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B90" s="7">
         <f t="shared" si="0"/>
         <v>43650</v>
@@ -2361,7 +2383,7 @@
         <v>1483.1305462166843</v>
       </c>
     </row>
-    <row r="91" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B91" s="7">
         <f t="shared" ref="B91:B146" si="1">B90+15</f>
         <v>43665</v>
@@ -2370,7 +2392,7 @@
         <v>1541.3556137339494</v>
       </c>
     </row>
-    <row r="92" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B92" s="7">
         <f t="shared" si="1"/>
         <v>43680</v>
@@ -2379,7 +2401,7 @@
         <v>1491.5831558670006</v>
       </c>
     </row>
-    <row r="93" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B93" s="7">
         <f t="shared" si="1"/>
         <v>43695</v>
@@ -2388,7 +2410,7 @@
         <v>1530.1479143460551</v>
       </c>
     </row>
-    <row r="94" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="94" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B94" s="7">
         <f t="shared" si="1"/>
         <v>43710</v>
@@ -2397,7 +2419,7 @@
         <v>1576.5520669759928</v>
       </c>
     </row>
-    <row r="95" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="95" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B95" s="7">
         <f t="shared" si="1"/>
         <v>43725</v>
@@ -2406,7 +2428,7 @@
         <v>1602.8396377079198</v>
       </c>
     </row>
-    <row r="96" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="96" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B96" s="7">
         <f t="shared" si="1"/>
         <v>43740</v>
@@ -2415,7 +2437,7 @@
         <v>1621.64031116812</v>
       </c>
     </row>
-    <row r="97" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B97" s="7">
         <f t="shared" si="1"/>
         <v>43755</v>
@@ -2424,7 +2446,7 @@
         <v>1666.831403093038</v>
       </c>
     </row>
-    <row r="98" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="98" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B98" s="7">
         <f t="shared" si="1"/>
         <v>43770</v>
@@ -2433,7 +2455,7 @@
         <v>1572.5012179677531</v>
       </c>
     </row>
-    <row r="99" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="99" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B99" s="7">
         <f t="shared" si="1"/>
         <v>43785</v>
@@ -2442,7 +2464,7 @@
         <v>1596.3117955128114</v>
       </c>
     </row>
-    <row r="100" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="100" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B100" s="7">
         <f t="shared" si="1"/>
         <v>43800</v>
@@ -2451,7 +2473,7 @@
         <v>1617.2074911293325</v>
       </c>
     </row>
-    <row r="101" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="101" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B101" s="7">
         <f t="shared" si="1"/>
         <v>43815</v>
@@ -2460,7 +2482,7 @@
         <v>1639.7155379252808</v>
       </c>
     </row>
-    <row r="102" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="102" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B102" s="7">
         <f t="shared" si="1"/>
         <v>43830</v>
@@ -2469,7 +2491,7 @@
         <v>1669.0137884368648</v>
       </c>
     </row>
-    <row r="103" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="103" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B103" s="7">
         <f t="shared" si="1"/>
         <v>43845</v>
@@ -2478,7 +2500,7 @@
         <v>1704.7734763937137</v>
       </c>
     </row>
-    <row r="104" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="104" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B104" s="7">
         <f t="shared" si="1"/>
         <v>43860</v>
@@ -2487,7 +2509,7 @@
         <v>1721.7231158678751</v>
       </c>
     </row>
-    <row r="105" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="105" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B105" s="7">
         <f t="shared" si="1"/>
         <v>43875</v>
@@ -2496,7 +2518,7 @@
         <v>1601.3054008782401</v>
       </c>
     </row>
-    <row r="106" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="106" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B106" s="7">
         <f t="shared" si="1"/>
         <v>43890</v>
@@ -2505,7 +2527,7 @@
         <v>1620.4898270435031</v>
       </c>
     </row>
-    <row r="107" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="107" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B107" s="7">
         <f t="shared" si="1"/>
         <v>43905</v>
@@ -2514,7 +2536,7 @@
         <v>1632.7798332395676</v>
       </c>
     </row>
-    <row r="108" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="108" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B108" s="7">
         <f t="shared" si="1"/>
         <v>43920</v>
@@ -2523,7 +2545,7 @@
         <v>1649.145077967486</v>
       </c>
     </row>
-    <row r="109" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="109" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B109" s="7">
         <f t="shared" si="1"/>
         <v>43935</v>
@@ -2532,7 +2554,7 @@
         <v>1671.4495178193251</v>
       </c>
     </row>
-    <row r="110" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="110" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B110" s="7">
         <f t="shared" si="1"/>
         <v>43950</v>
@@ -2541,7 +2563,7 @@
         <v>1693.9399090570441</v>
       </c>
     </row>
-    <row r="111" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="111" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B111" s="7">
         <f t="shared" si="1"/>
         <v>43965</v>
@@ -2550,7 +2572,7 @@
         <v>1539.7720457046748</v>
       </c>
     </row>
-    <row r="112" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="112" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B112" s="7">
         <f t="shared" si="1"/>
         <v>43980</v>
@@ -2559,7 +2581,7 @@
         <v>1558.5115652939269</v>
       </c>
     </row>
-    <row r="113" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="113" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B113" s="7">
         <f t="shared" si="1"/>
         <v>43995</v>
@@ -2568,7 +2590,7 @@
         <v>1573.2632442473425</v>
       </c>
     </row>
-    <row r="114" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="114" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B114" s="7">
         <f t="shared" si="1"/>
         <v>44010</v>
@@ -2577,7 +2599,7 @@
         <v>1592.1479094859324</v>
       </c>
     </row>
-    <row r="115" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="115" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B115" s="7">
         <f t="shared" si="1"/>
         <v>44025</v>
@@ -2586,7 +2608,7 @@
         <v>1599.1224529891049</v>
       </c>
     </row>
-    <row r="116" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="116" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B116" s="7">
         <f t="shared" si="1"/>
         <v>44040</v>
@@ -2595,7 +2617,7 @@
         <v>1615.786301334294</v>
       </c>
     </row>
-    <row r="117" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="117" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B117" s="7">
         <f t="shared" si="1"/>
         <v>44055</v>
@@ -2604,7 +2626,7 @@
         <v>1411.0080210997874</v>
       </c>
     </row>
-    <row r="118" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="118" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B118" s="7">
         <f t="shared" si="1"/>
         <v>44070</v>
@@ -2613,7 +2635,7 @@
         <v>1424.2263678418358</v>
       </c>
     </row>
-    <row r="119" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="119" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B119" s="7">
         <f t="shared" si="1"/>
         <v>44085</v>
@@ -2622,7 +2644,7 @@
         <v>1435.6297353612122</v>
       </c>
     </row>
-    <row r="120" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="120" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B120" s="7">
         <f t="shared" si="1"/>
         <v>44100</v>
@@ -2631,7 +2653,7 @@
         <v>1444.5939620911495</v>
       </c>
     </row>
-    <row r="121" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="121" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B121" s="7">
         <f t="shared" si="1"/>
         <v>44115</v>
@@ -2640,7 +2662,7 @@
         <v>1454.9311122201282</v>
       </c>
     </row>
-    <row r="122" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="122" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B122" s="7">
         <f t="shared" si="1"/>
         <v>44130</v>
@@ -2649,7 +2671,7 @@
         <v>1473.7640670957662</v>
       </c>
     </row>
-    <row r="123" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="123" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B123" s="7">
         <f t="shared" si="1"/>
         <v>44145</v>
@@ -2658,7 +2680,7 @@
         <v>1243.1443655145872</v>
       </c>
     </row>
-    <row r="124" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="124" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B124" s="7">
         <f t="shared" si="1"/>
         <v>44160</v>
@@ -2667,7 +2689,7 @@
         <v>1246.458772956863</v>
       </c>
     </row>
-    <row r="125" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="125" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B125" s="7">
         <f t="shared" si="1"/>
         <v>44175</v>
@@ -2676,7 +2698,7 @@
         <v>1250.1801245204556</v>
       </c>
     </row>
-    <row r="126" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="126" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B126" s="7">
         <f t="shared" si="1"/>
         <v>44190</v>
@@ -2685,7 +2707,7 @@
         <v>1258.4100830775412</v>
       </c>
     </row>
-    <row r="127" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="127" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B127" s="7">
         <f t="shared" si="1"/>
         <v>44205</v>
@@ -2694,7 +2716,7 @@
         <v>1268.7283489824581</v>
       </c>
     </row>
-    <row r="128" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="128" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B128" s="7">
         <f t="shared" si="1"/>
         <v>44220</v>
@@ -2703,7 +2725,7 @@
         <v>1281.005602806465</v>
       </c>
     </row>
-    <row r="129" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="129" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B129" s="7">
         <f t="shared" si="1"/>
         <v>44235</v>
@@ -2712,7 +2734,7 @@
         <v>1029.7735675214969</v>
       </c>
     </row>
-    <row r="130" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="130" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B130" s="7">
         <f t="shared" si="1"/>
         <v>44250</v>
@@ -2721,7 +2743,7 @@
         <v>1037.1564459421438</v>
       </c>
     </row>
-    <row r="131" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="131" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B131" s="7">
         <f t="shared" si="1"/>
         <v>44265</v>
@@ -2730,7 +2752,7 @@
         <v>1039.5975938678268</v>
       </c>
     </row>
-    <row r="132" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="132" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B132" s="7">
         <f t="shared" si="1"/>
         <v>44280</v>
@@ -2739,7 +2761,7 @@
         <v>1045.1321244180285</v>
       </c>
     </row>
-    <row r="133" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="133" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B133" s="7">
         <f t="shared" si="1"/>
         <v>44295</v>
@@ -2748,7 +2770,7 @@
         <v>1048.2314218646941</v>
       </c>
     </row>
-    <row r="134" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="134" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B134" s="7">
         <f t="shared" si="1"/>
         <v>44310</v>
@@ -2757,7 +2779,7 @@
         <v>1059.2601865500501</v>
       </c>
     </row>
-    <row r="135" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="135" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B135" s="7">
         <f t="shared" si="1"/>
         <v>44325</v>
@@ -2766,7 +2788,7 @@
         <v>784.38358582574813</v>
       </c>
     </row>
-    <row r="136" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="136" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B136" s="7">
         <f t="shared" si="1"/>
         <v>44340</v>
@@ -2775,7 +2797,7 @@
         <v>784.51568238942559</v>
       </c>
     </row>
-    <row r="137" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="137" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B137" s="7">
         <f t="shared" si="1"/>
         <v>44355</v>
@@ -2784,7 +2806,7 @@
         <v>784.59397650783626</v>
       </c>
     </row>
-    <row r="138" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="138" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B138" s="7">
         <f t="shared" si="1"/>
         <v>44370</v>
@@ -2793,7 +2815,7 @@
         <v>785.95759562746662</v>
       </c>
     </row>
-    <row r="139" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="139" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B139" s="7">
         <f t="shared" si="1"/>
         <v>44385</v>
@@ -2802,7 +2824,7 @@
         <v>787.44073155746662</v>
       </c>
     </row>
-    <row r="140" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="140" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B140" s="7">
         <f t="shared" si="1"/>
         <v>44400</v>
@@ -2811,7 +2833,7 @@
         <v>789.2823395128255</v>
       </c>
     </row>
-    <row r="141" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="141" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B141" s="7">
         <f t="shared" si="1"/>
         <v>44415</v>
@@ -2820,7 +2842,7 @@
         <v>485.32972976694367</v>
       </c>
     </row>
-    <row r="142" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="142" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B142" s="7">
         <f t="shared" si="1"/>
         <v>44430</v>
@@ -2829,7 +2851,7 @@
         <v>479.95788106267059</v>
       </c>
     </row>
-    <row r="143" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="143" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B143" s="7">
         <f t="shared" si="1"/>
         <v>44445</v>
@@ -2838,7 +2860,7 @@
         <v>473.81021110626386</v>
       </c>
     </row>
-    <row r="144" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="144" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B144" s="7">
         <f t="shared" si="1"/>
         <v>44460</v>
@@ -2847,7 +2869,7 @@
         <v>469.43690998874439</v>
       </c>
     </row>
-    <row r="145" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="145" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B145" s="7">
         <f t="shared" si="1"/>
         <v>44475</v>
@@ -2856,7 +2878,7 @@
         <v>464.80849303355564</v>
       </c>
     </row>
-    <row r="146" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="146" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B146" s="7">
         <f t="shared" si="1"/>
         <v>44490</v>
@@ -2879,15 +2901,15 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="35.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.88671875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:7" ht="15" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
@@ -2901,7 +2923,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:7" ht="15" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
@@ -2915,7 +2937,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:7" ht="15" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>3</v>
       </c>
@@ -2923,7 +2945,7 @@
         <v>8.9999999999999993E-3</v>
       </c>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:7" ht="15" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>4</v>
       </c>
@@ -2938,7 +2960,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:7" ht="15" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>5</v>
       </c>
@@ -2952,7 +2974,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:7" ht="15" x14ac:dyDescent="0.25">
       <c r="F7" s="7">
         <v>46327</v>
       </c>
@@ -2965,7 +2987,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:7" ht="15" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="str">
         <f>_xll.QSA.CreateHWModelDemo(C2,C3,C4,C5,C6)</f>
         <v>HWDemo.09:10:26-124</v>

</xml_diff>

<commit_message>
Use SerializableViaName for Excel converters.
</commit_message>
<xml_diff>
--- a/ExcelExamples/BermudanSwaption.xlsx
+++ b/ExcelExamples/BermudanSwaption.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="37">
   <si>
     <t>name</t>
   </si>
@@ -54,9 +54,6 @@
     <t>QSA.CreateHWModelDemo</t>
   </si>
   <si>
-    <t>JIBAR3M</t>
-  </si>
-  <si>
     <t>startDate</t>
   </si>
   <si>
@@ -124,6 +121,12 @@
   </si>
   <si>
     <t>QSA.GetResults</t>
+  </si>
+  <si>
+    <t>ZAR.JIBAR.3M</t>
+  </si>
+  <si>
+    <t>jibar</t>
   </si>
 </sst>
 </file>
@@ -282,7 +285,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Product&amp;EPE'!$B$25:$B$146</c:f>
+              <c:f>'Product&amp;EPE'!$B$26:$B$147</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm\-yy</c:formatCode>
                 <c:ptCount val="122"/>
@@ -657,7 +660,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Product&amp;EPE'!$C$25:$C$146</c:f>
+              <c:f>'Product&amp;EPE'!$C$26:$C$147</c:f>
               <c:numCache>
                 <c:formatCode>#,##0.00</c:formatCode>
                 <c:ptCount val="122"/>
@@ -665,19 +668,19 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>0.64653070893433173</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>0.49706959177944371</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.27067610339485509</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.58766449057314163</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.33330954272205415</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0</c:v>
@@ -686,346 +689,346 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
+                  <c:v>0.28674479930411617</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.0513201690382024</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10.437653922229206</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>9.1277433160860628</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>6.7256824783779727</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.4382008922410932</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>4.0788148116053273</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>5.4033693396362823</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.170415370404674</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>3.858765170336238</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.92652239358102595</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.2222116728751741</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.76871915779433708</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>3.686670875798133</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>3.9056508250153863</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2.6516464586633761</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.23493298499122958</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2.2695345985447859</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>3.2778873891288183</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2.0555395850165294</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1.4067000288659204</c:v>
+                </c:pt>
+                <c:pt idx="29">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="30">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.16095383044728206</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>2.287870045080393</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0.45330458066640766</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>2.4650942759317331</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>0.3435804514881779</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>6.4394953071166761</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>15.432070455697964</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>12.606054757416631</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>12.457713634014713</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>10.686992351896832</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>12.195249894161828</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>11.294221892745716</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>9.4098841146912946</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>3.7370042565768635</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>3.884872441489903</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>6.6806074316484079</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>5.2818599662227257</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>5.0306173714740856</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>5.0769801450758747</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>5.5724967934043761</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>4.1951096947929578</c:v>
-                </c:pt>
                 <c:pt idx="31">
-                  <c:v>2.3875447715824505</c:v>
+                  <c:v>1.2844484155122853</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0</c:v>
+                  <c:v>1.0690362323696481</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0</c:v>
+                  <c:v>1.6533402775090549</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0.91050756464516125</c:v>
+                  <c:v>0.84725350097536067</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>14.207884605877252</c:v>
+                  <c:v>1.5555048134169525</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>20.08437522096602</c:v>
+                  <c:v>0.12050822542382689</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>37.248532479395813</c:v>
+                  <c:v>19.24015801632299</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>93.48921668815882</c:v>
+                  <c:v>44.466884831654596</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>140.07363864430579</c:v>
+                  <c:v>123.58747827563938</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>219.48755143385762</c:v>
+                  <c:v>183.35237069607416</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>257.50144333128566</c:v>
+                  <c:v>203.09191307309914</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>287.58051598618971</c:v>
+                  <c:v>242.41707847580653</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>345.71963364839581</c:v>
+                  <c:v>287.21049311362412</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>418.9177123749684</c:v>
+                  <c:v>327.95712817208903</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>484.14215321555065</c:v>
+                  <c:v>360.19137260029436</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>534.1174176641432</c:v>
+                  <c:v>444.69735654145973</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>596.81580883009633</c:v>
+                  <c:v>565.86072499217551</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>641.85927527087085</c:v>
+                  <c:v>597.03613590149962</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>646.78994567192058</c:v>
+                  <c:v>635.73648191409018</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>677.83475841021925</c:v>
+                  <c:v>686.74653649226775</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>711.35828379384827</c:v>
+                  <c:v>709.39020323935006</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>776.4477956452115</c:v>
+                  <c:v>828.84981916110223</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>837.04067831908981</c:v>
+                  <c:v>832.35594069114131</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>903.93467461764351</c:v>
+                  <c:v>913.46021052844321</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>946.65568584893754</c:v>
+                  <c:v>893.06849684777615</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>1012.7239831227166</c:v>
+                  <c:v>955.7869342919962</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>1017.3593473935928</c:v>
+                  <c:v>1010.884074190806</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>1087.4820314195929</c:v>
+                  <c:v>1027.4566329956604</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>1160.9007706132393</c:v>
+                  <c:v>1120.4545429487562</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>1236.2772736675643</c:v>
+                  <c:v>1141.3637680050983</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>1243.7606195230567</c:v>
+                  <c:v>1140.9472365844526</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>1292.5399230650826</c:v>
+                  <c:v>1185.8912989073822</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>1361.4491862225104</c:v>
+                  <c:v>1199.2932153274462</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>1414.2334161517551</c:v>
+                  <c:v>1240.0842011242521</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>1483.1305462166843</c:v>
+                  <c:v>1243.908485019899</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>1541.3556137339494</c:v>
+                  <c:v>1288.299242688923</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>1491.5831558670006</c:v>
+                  <c:v>1224.0748474829259</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>1530.1479143460551</c:v>
+                  <c:v>1282.2161145644516</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>1576.5520669759928</c:v>
+                  <c:v>1303.953812402199</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>1602.8396377079198</c:v>
+                  <c:v>1329.3937054089033</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>1621.64031116812</c:v>
+                  <c:v>1376.4269221127595</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>1666.831403093038</c:v>
+                  <c:v>1393.6288149925208</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>1572.5012179677531</c:v>
+                  <c:v>1325.1575338148511</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>1596.3117955128114</c:v>
+                  <c:v>1349.8462039338719</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>1617.2074911293325</c:v>
+                  <c:v>1377.1401349694709</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>1639.7155379252808</c:v>
+                  <c:v>1403.2077171059793</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>1669.0137884368648</c:v>
+                  <c:v>1404.1814086812417</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>1704.7734763937137</c:v>
+                  <c:v>1435.7319990007541</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>1721.7231158678751</c:v>
+                  <c:v>1464.4938767803901</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>1601.3054008782401</c:v>
+                  <c:v>1322.213080578701</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>1620.4898270435031</c:v>
+                  <c:v>1349.9357161289024</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>1632.7798332395676</c:v>
+                  <c:v>1366.3364846764123</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>1649.145077967486</c:v>
+                  <c:v>1379.6189207042255</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>1671.4495178193251</c:v>
+                  <c:v>1428.1226735119735</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>1693.9399090570441</c:v>
+                  <c:v>1445.7079871938527</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>1539.7720457046748</c:v>
+                  <c:v>1279.8674474269685</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>1558.5115652939269</c:v>
+                  <c:v>1287.9056745528653</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>1573.2632442473425</c:v>
+                  <c:v>1296.6593342879682</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>1592.1479094859324</c:v>
+                  <c:v>1313.9701291870786</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>1599.1224529891049</c:v>
+                  <c:v>1337.5356523283872</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>1615.786301334294</c:v>
+                  <c:v>1348.3240250964293</c:v>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>1411.0080210997874</c:v>
+                  <c:v>1162.8244231391045</c:v>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>1424.2263678418358</c:v>
+                  <c:v>1165.2286023690199</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>1435.6297353612122</c:v>
+                  <c:v>1166.1137329123385</c:v>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>1444.5939620911495</c:v>
+                  <c:v>1174.9505611698819</c:v>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>1454.9311122201282</c:v>
+                  <c:v>1187.1988058998409</c:v>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>1473.7640670957662</c:v>
+                  <c:v>1198.7151861639536</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>1243.1443655145872</c:v>
+                  <c:v>990.48320610803239</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>1246.458772956863</c:v>
+                  <c:v>991.71025151818696</c:v>
                 </c:pt>
                 <c:pt idx="100">
-                  <c:v>1250.1801245204556</c:v>
+                  <c:v>1004.7614445840968</c:v>
                 </c:pt>
                 <c:pt idx="101">
-                  <c:v>1258.4100830775412</c:v>
+                  <c:v>1007.2397743879393</c:v>
                 </c:pt>
                 <c:pt idx="102">
-                  <c:v>1268.7283489824581</c:v>
+                  <c:v>1020.5489770455223</c:v>
                 </c:pt>
                 <c:pt idx="103">
-                  <c:v>1281.005602806465</c:v>
+                  <c:v>1030.2241902087057</c:v>
                 </c:pt>
                 <c:pt idx="104">
-                  <c:v>1029.7735675214969</c:v>
+                  <c:v>801.98707976094056</c:v>
                 </c:pt>
                 <c:pt idx="105">
-                  <c:v>1037.1564459421438</c:v>
+                  <c:v>804.93363602883016</c:v>
                 </c:pt>
                 <c:pt idx="106">
-                  <c:v>1039.5975938678268</c:v>
+                  <c:v>808.88846947213813</c:v>
                 </c:pt>
                 <c:pt idx="107">
-                  <c:v>1045.1321244180285</c:v>
+                  <c:v>814.11579808135559</c:v>
                 </c:pt>
                 <c:pt idx="108">
-                  <c:v>1048.2314218646941</c:v>
+                  <c:v>822.31900902957466</c:v>
                 </c:pt>
                 <c:pt idx="109">
-                  <c:v>1059.2601865500501</c:v>
+                  <c:v>823.41895797462337</c:v>
                 </c:pt>
                 <c:pt idx="110">
-                  <c:v>784.38358582574813</c:v>
+                  <c:v>577.98199238304335</c:v>
                 </c:pt>
                 <c:pt idx="111">
-                  <c:v>784.51568238942559</c:v>
+                  <c:v>577.89956794405691</c:v>
                 </c:pt>
                 <c:pt idx="112">
-                  <c:v>784.59397650783626</c:v>
+                  <c:v>578.26982912862229</c:v>
                 </c:pt>
                 <c:pt idx="113">
-                  <c:v>785.95759562746662</c:v>
+                  <c:v>578.57441240430626</c:v>
                 </c:pt>
                 <c:pt idx="114">
-                  <c:v>787.44073155746662</c:v>
+                  <c:v>578.92070392709491</c:v>
                 </c:pt>
                 <c:pt idx="115">
-                  <c:v>789.2823395128255</c:v>
+                  <c:v>578.84052317282317</c:v>
                 </c:pt>
                 <c:pt idx="116">
-                  <c:v>485.32972976694367</c:v>
+                  <c:v>306.59207131272933</c:v>
                 </c:pt>
                 <c:pt idx="117">
-                  <c:v>479.95788106267059</c:v>
+                  <c:v>303.14322533324707</c:v>
                 </c:pt>
                 <c:pt idx="118">
-                  <c:v>473.81021110626386</c:v>
+                  <c:v>299.3380272572042</c:v>
                 </c:pt>
                 <c:pt idx="119">
-                  <c:v>469.43690998874439</c:v>
+                  <c:v>293.79157339572407</c:v>
                 </c:pt>
                 <c:pt idx="120">
-                  <c:v>464.80849303355564</c:v>
+                  <c:v>289.7923352371858</c:v>
                 </c:pt>
                 <c:pt idx="121">
-                  <c:v>459.815138814985</c:v>
+                  <c:v>285.63079090851278</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1042,11 +1045,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="265243264"/>
-        <c:axId val="265253248"/>
+        <c:axId val="201545984"/>
+        <c:axId val="201580544"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="265243264"/>
+        <c:axId val="201545984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1056,14 +1059,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="265253248"/>
+        <c:crossAx val="201580544"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="265253248"/>
+        <c:axId val="201580544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1074,7 +1077,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="265243264"/>
+        <c:crossAx val="201545984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1103,7 +1106,7 @@
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1415,10 +1418,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:E27"/>
+  <dimension ref="B2:E28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1431,7 +1434,7 @@
   <sheetData>
     <row r="2" spans="2:5" ht="15" x14ac:dyDescent="0.25">
       <c r="E2" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="2:5" ht="15" x14ac:dyDescent="0.25">
@@ -1441,7 +1444,7 @@
     </row>
     <row r="4" spans="2:5" ht="15" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C4" s="4" t="b">
         <v>0</v>
@@ -1452,7 +1455,7 @@
     </row>
     <row r="5" spans="2:5" ht="15" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C5" s="7">
         <v>42675</v>
@@ -1463,10 +1466,10 @@
     </row>
     <row r="6" spans="2:5" ht="15" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>14</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>15</v>
       </c>
       <c r="E6" s="7">
         <v>44136</v>
@@ -1474,7 +1477,7 @@
     </row>
     <row r="7" spans="2:5" ht="15" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C7" s="8">
         <v>7.0000000000000007E-2</v>
@@ -1482,7 +1485,7 @@
     </row>
     <row r="8" spans="2:5" ht="15" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C8" s="4" t="b">
         <v>1</v>
@@ -1490,27 +1493,23 @@
     </row>
     <row r="9" spans="2:5" ht="15" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C9" s="9">
         <v>1000000</v>
       </c>
     </row>
-    <row r="11" spans="2:5" ht="21" x14ac:dyDescent="0.35">
-      <c r="C11" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="12" spans="2:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="B12" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="D12" s="3" t="str">
-        <f>_xll.QSA.CreateZARBermudanSwaption(C12,E3,C4,C5,C6,C7,C8,C9)</f>
-        <v>Swaption1Ex.09:10:26-122</v>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B10" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="C12" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="2:5" ht="15" x14ac:dyDescent="0.25">
@@ -1518,11 +1517,11 @@
         <v>0</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D13" s="3" t="str">
-        <f>_xll.QSA.CreateZARBermudanSwaption(C13,E3:E4,C4,C5,C6,C7,C8,C9)</f>
-        <v>Swaption2Ex.09:10:26-119</v>
+        <f ca="1">_xll.QSA.CreateZARBermudanSwaption(C13,$E$3:E3,$C$4,$C$5,$C$6,$C$7,$C$8,$C$9,$C$10)</f>
+        <v>Swaption1Ex.21:17:07-30</v>
       </c>
     </row>
     <row r="14" spans="2:5" ht="15" x14ac:dyDescent="0.25">
@@ -1530,11 +1529,11 @@
         <v>0</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D14" s="3" t="str">
-        <f>_xll.QSA.CreateZARBermudanSwaption(C14,E3:E5,C4,C5,C6,C7,C8,C9)</f>
-        <v>Swaption3Ex.09:10:26-120</v>
+        <f ca="1">_xll.QSA.CreateZARBermudanSwaption(C14,$E$3:E4,$C$4,$C$5,$C$6,$C$7,$C$8,$C$9,$C$10)</f>
+        <v>Swaption2Ex.21:17:07-29</v>
       </c>
     </row>
     <row r="15" spans="2:5" ht="15" x14ac:dyDescent="0.25">
@@ -1542,93 +1541,105 @@
         <v>0</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D15" s="3" t="str">
-        <f>_xll.QSA.CreateZARBermudanSwaption(C15,E3:E6,C4,C5,C6,C7,C8,C9)</f>
-        <v>Swaption4Ex.09:10:26-121</v>
-      </c>
-    </row>
-    <row r="17" spans="2:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="B17" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C17" s="10">
-        <f>Model!F6</f>
-        <v>42675</v>
+        <f ca="1">_xll.QSA.CreateZARBermudanSwaption(C15,$E$3:E5,$C$4,$C$5,$C$6,$C$7,$C$8,$C$9,$C$10)</f>
+        <v>Swaption3Ex.21:17:07-31</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="B16" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D16" s="3" t="str">
+        <f ca="1">_xll.QSA.CreateZARBermudanSwaption(C16,$E$3:E6,$C$4,$C$5,$C$6,$C$7,$C$8,$C$9,$C$10)</f>
+        <v>Swaption4Ex.21:17:07-32</v>
       </c>
     </row>
     <row r="18" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B18" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C18" s="6" t="str">
-        <f>Model!B9</f>
-        <v>HWDemo.09:10:26-124</v>
+        <v>20</v>
+      </c>
+      <c r="C18" s="10">
+        <f ca="1">Model!F6</f>
+        <v>42675</v>
       </c>
     </row>
     <row r="19" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B19" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C19" s="4">
+        <v>22</v>
+      </c>
+      <c r="C19" s="6" t="str">
+        <f ca="1">Model!B9</f>
+        <v>HWDemo.21:15:14-7</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B20" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C20" s="4">
         <v>5000</v>
-      </c>
-    </row>
-    <row r="21" spans="2:3" ht="21" x14ac:dyDescent="0.4">
-      <c r="C21" s="1" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="22" spans="2:3" ht="21" x14ac:dyDescent="0.4">
       <c r="C22" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="23" spans="2:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="C23" t="str">
-        <f ca="1">_xll.QSA.GetAvailableResults(B24)</f>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" ht="21" x14ac:dyDescent="0.4">
+      <c r="C23" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="C24" t="str">
+        <f ca="1">_xll.QSA.GetAvailableResults(B25)</f>
         <v>value</v>
       </c>
     </row>
-    <row r="24" spans="2:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="B24" s="3" t="str">
-        <f>_xll.QSA.Value(C12&amp;"Value",D12,$C$17,$C$18,$C$19)</f>
-        <v>Swaption1ExValue.09:10:26-125</v>
-      </c>
-      <c r="C24" s="11">
-        <f>_xll.QSA.GetResults(B24,"value")</f>
-        <v>-9597.2890686645351</v>
-      </c>
-    </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B25" s="3" t="str">
-        <f>_xll.QSA.Value(C13&amp;"Value",D13,$C$17,$C$18,$C$19)</f>
-        <v>Swaption2ExValue.09:10:28-128</v>
+        <f ca="1">_xll.QSA.Value(C13&amp;"Value",D13,$C$18,$C$19,$C$20)</f>
+        <v>Swaption1ExValue.21:17:09-35</v>
       </c>
       <c r="C25" s="11">
-        <f>_xll.QSA.GetResults(B25,"value")</f>
-        <v>-11978.432212997121</v>
+        <f ca="1">_xll.QSA.GetResults(B25,"value")</f>
+        <v>-9253.0687187579679</v>
       </c>
     </row>
     <row r="26" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B26" s="3" t="str">
-        <f>_xll.QSA.Value(C14&amp;"Value",D14,$C$17,$C$18,$C$19)</f>
-        <v>Swaption3ExValue.09:10:27-127</v>
+        <f ca="1">_xll.QSA.Value(C14&amp;"Value",D14,$C$18,$C$19,$C$20)</f>
+        <v>Swaption2ExValue.21:17:08-34</v>
       </c>
       <c r="C26" s="11">
-        <f>_xll.QSA.GetResults(B26,"value")</f>
-        <v>-12965.151497549465</v>
+        <f ca="1">_xll.QSA.GetResults(B26,"value")</f>
+        <v>-11759.643679972569</v>
       </c>
     </row>
     <row r="27" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B27" s="3" t="str">
-        <f>_xll.QSA.Value(C15&amp;"Value",D15,$C$17,$C$18,$C$19)</f>
-        <v>Swaption4ExValue.09:10:27-126</v>
+        <f ca="1">_xll.QSA.Value(C15&amp;"Value",D15,$C$18,$C$19,$C$20)</f>
+        <v>Swaption3ExValue.21:17:08-33</v>
       </c>
       <c r="C27" s="11">
-        <f>_xll.QSA.GetResults(B27,"value")</f>
-        <v>-13296.063937555664</v>
+        <f ca="1">_xll.QSA.GetResults(B27,"value")</f>
+        <v>-12759.910741854084</v>
+      </c>
+    </row>
+    <row r="28" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B28" s="3" t="str">
+        <f ca="1">_xll.QSA.Value(C16&amp;"Value",D16,$C$18,$C$19,$C$20)</f>
+        <v>Swaption4ExValue.21:17:09-36</v>
+      </c>
+      <c r="C28" s="11">
+        <f ca="1">_xll.QSA.GetResults(B28,"value")</f>
+        <v>-13074.56016657424</v>
       </c>
     </row>
   </sheetData>
@@ -1638,10 +1649,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:E146"/>
+  <dimension ref="B2:E147"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F64" sqref="F64"/>
+      <selection activeCell="B10" sqref="B10:C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1656,10 +1667,10 @@
         <v>0</v>
       </c>
       <c r="C2" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>26</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="3" spans="2:5" ht="15" x14ac:dyDescent="0.25">
@@ -1669,7 +1680,7 @@
     </row>
     <row r="4" spans="2:5" ht="15" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C4" s="4" t="b">
         <v>0</v>
@@ -1680,7 +1691,7 @@
     </row>
     <row r="5" spans="2:5" ht="15" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C5" s="7">
         <v>42675</v>
@@ -1691,10 +1702,10 @@
     </row>
     <row r="6" spans="2:5" ht="15" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>14</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>15</v>
       </c>
       <c r="E6" s="7">
         <v>44136</v>
@@ -1702,7 +1713,7 @@
     </row>
     <row r="7" spans="2:5" ht="15" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C7" s="8">
         <v>7.0000000000000007E-2</v>
@@ -1710,7 +1721,7 @@
     </row>
     <row r="8" spans="2:5" ht="15" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C8" s="4" t="b">
         <v>1</v>
@@ -1718,108 +1729,107 @@
     </row>
     <row r="9" spans="2:5" ht="15" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C9" s="9">
         <v>1000000</v>
       </c>
     </row>
-    <row r="11" spans="2:5" ht="21" x14ac:dyDescent="0.35">
-      <c r="B11" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="12" spans="2:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="B12" s="3" t="str">
-        <f>_xll.QSA.CreateZARBermudanSwaption(C2,E3:E4,C4,C5,C6,C7,C8,C9)</f>
-        <v>BermudanSwaption0001.09:10:26-118</v>
-      </c>
-    </row>
-    <row r="15" spans="2:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="B15" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>20</v>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B10" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="B12" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="B13" s="3" t="str">
+        <f>_xll.QSA.CreateZARBermudanSwaption(C2,E3:E4,C4,C5,C6,C7,C8,C9,C10)</f>
+        <v>BermudanSwaption0001.21:15:14-5</v>
       </c>
     </row>
     <row r="16" spans="2:5" ht="15" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C16" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C16" s="6" t="str">
-        <f>B12</f>
-        <v>BermudanSwaption0001.09:10:26-118</v>
-      </c>
-    </row>
-    <row r="19" spans="2:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="B19" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C19" s="10">
+    </row>
+    <row r="17" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B17" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" s="6" t="str">
+        <f>B13</f>
+        <v>BermudanSwaption0001.21:15:14-5</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B20" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C20" s="10">
         <f>Model!F6</f>
         <v>42675</v>
       </c>
     </row>
-    <row r="20" spans="2:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="B20" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C20" s="6" t="str">
-        <f>Model!B9</f>
-        <v>HWDemo.09:10:26-124</v>
-      </c>
-    </row>
     <row r="21" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B21" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C21" s="6" t="str">
+        <f>Model!B9</f>
+        <v>HWDemo.21:15:14-7</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B22" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C22" s="4">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" ht="21" x14ac:dyDescent="0.35">
+      <c r="B24" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C21" s="4">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="23" spans="2:3" ht="21" x14ac:dyDescent="0.35">
-      <c r="B23" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="24" spans="2:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="B24" s="2" t="s">
-        <v>22</v>
-      </c>
     </row>
     <row r="25" spans="2:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="B25" s="7">
-        <f>C19</f>
-        <v>42675</v>
-      </c>
-      <c r="C25" s="11">
-        <f t="array" ref="C25:C146">_xll.QSA.EPE(C16,C19,B25:B146,C20,C21)</f>
-        <v>0</v>
+      <c r="B25" s="2" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="26" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B26" s="7">
-        <f>B25+15</f>
-        <v>42690</v>
+        <f>C20</f>
+        <v>42675</v>
       </c>
       <c r="C26" s="11">
+        <f t="array" ref="C26:C147">_xll.QSA.EPE(C17,C20,B26:B147,C21,C22)</f>
         <v>0</v>
       </c>
     </row>
     <row r="27" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B27" s="7">
-        <f t="shared" ref="B27:B90" si="0">B26+15</f>
-        <v>42705</v>
+        <f>B26+15</f>
+        <v>42690</v>
       </c>
       <c r="C27" s="11">
-        <v>0</v>
+        <v>0.64653070893433173</v>
       </c>
     </row>
     <row r="28" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B28" s="7">
-        <f t="shared" si="0"/>
-        <v>42720</v>
+        <f t="shared" ref="B28:B91" si="0">B27+15</f>
+        <v>42705</v>
       </c>
       <c r="C28" s="11">
         <v>0</v>
@@ -1828,25 +1838,25 @@
     <row r="29" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B29" s="7">
         <f t="shared" si="0"/>
-        <v>42735</v>
+        <v>42720</v>
       </c>
       <c r="C29" s="11">
-        <v>0.58766449057314163</v>
+        <v>0.49706959177944371</v>
       </c>
     </row>
     <row r="30" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B30" s="7">
         <f t="shared" si="0"/>
+        <v>42735</v>
+      </c>
+      <c r="C30" s="11">
+        <v>0.27067610339485509</v>
+      </c>
+    </row>
+    <row r="31" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B31" s="7">
+        <f t="shared" si="0"/>
         <v>42750</v>
-      </c>
-      <c r="C30" s="11">
-        <v>0.33330954272205415</v>
-      </c>
-    </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B31" s="7">
-        <f t="shared" si="0"/>
-        <v>42765</v>
       </c>
       <c r="C31" s="11">
         <v>0</v>
@@ -1855,7 +1865,7 @@
     <row r="32" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B32" s="7">
         <f t="shared" si="0"/>
-        <v>42780</v>
+        <v>42765</v>
       </c>
       <c r="C32" s="11">
         <v>0</v>
@@ -1864,7 +1874,7 @@
     <row r="33" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B33" s="7">
         <f t="shared" si="0"/>
-        <v>42795</v>
+        <v>42780</v>
       </c>
       <c r="C33" s="11">
         <v>0</v>
@@ -1873,1018 +1883,1027 @@
     <row r="34" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B34" s="7">
         <f t="shared" si="0"/>
-        <v>42810</v>
+        <v>42795</v>
       </c>
       <c r="C34" s="11">
-        <v>0</v>
+        <v>0.28674479930411617</v>
       </c>
     </row>
     <row r="35" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B35" s="7">
         <f t="shared" si="0"/>
-        <v>42825</v>
+        <v>42810</v>
       </c>
       <c r="C35" s="11">
-        <v>0.16095383044728206</v>
+        <v>1.0513201690382024</v>
       </c>
     </row>
     <row r="36" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B36" s="7">
         <f t="shared" si="0"/>
-        <v>42840</v>
+        <v>42825</v>
       </c>
       <c r="C36" s="11">
-        <v>2.287870045080393</v>
+        <v>10.437653922229206</v>
       </c>
     </row>
     <row r="37" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B37" s="7">
         <f t="shared" si="0"/>
-        <v>42855</v>
+        <v>42840</v>
       </c>
       <c r="C37" s="11">
-        <v>0.45330458066640766</v>
+        <v>9.1277433160860628</v>
       </c>
     </row>
     <row r="38" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B38" s="7">
         <f t="shared" si="0"/>
-        <v>42870</v>
+        <v>42855</v>
       </c>
       <c r="C38" s="11">
-        <v>2.4650942759317331</v>
+        <v>6.7256824783779727</v>
       </c>
     </row>
     <row r="39" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B39" s="7">
         <f t="shared" si="0"/>
-        <v>42885</v>
+        <v>42870</v>
       </c>
       <c r="C39" s="11">
-        <v>0.3435804514881779</v>
+        <v>1.4382008922410932</v>
       </c>
     </row>
     <row r="40" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B40" s="7">
         <f t="shared" si="0"/>
-        <v>42900</v>
+        <v>42885</v>
       </c>
       <c r="C40" s="11">
-        <v>6.4394953071166761</v>
+        <v>4.0788148116053273</v>
       </c>
     </row>
     <row r="41" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B41" s="7">
         <f t="shared" si="0"/>
-        <v>42915</v>
+        <v>42900</v>
       </c>
       <c r="C41" s="11">
-        <v>15.432070455697964</v>
+        <v>5.4033693396362823</v>
       </c>
     </row>
     <row r="42" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B42" s="7">
         <f t="shared" si="0"/>
-        <v>42930</v>
+        <v>42915</v>
       </c>
       <c r="C42" s="11">
-        <v>12.606054757416631</v>
+        <v>1.170415370404674</v>
       </c>
     </row>
     <row r="43" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B43" s="7">
         <f t="shared" si="0"/>
-        <v>42945</v>
+        <v>42930</v>
       </c>
       <c r="C43" s="11">
-        <v>12.457713634014713</v>
+        <v>3.858765170336238</v>
       </c>
     </row>
     <row r="44" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B44" s="7">
         <f t="shared" si="0"/>
-        <v>42960</v>
+        <v>42945</v>
       </c>
       <c r="C44" s="11">
-        <v>10.686992351896832</v>
+        <v>0.92652239358102595</v>
       </c>
     </row>
     <row r="45" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B45" s="7">
         <f t="shared" si="0"/>
-        <v>42975</v>
+        <v>42960</v>
       </c>
       <c r="C45" s="11">
-        <v>12.195249894161828</v>
+        <v>0.2222116728751741</v>
       </c>
     </row>
     <row r="46" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B46" s="7">
         <f t="shared" si="0"/>
-        <v>42990</v>
+        <v>42975</v>
       </c>
       <c r="C46" s="11">
-        <v>11.294221892745716</v>
+        <v>0.76871915779433708</v>
       </c>
     </row>
     <row r="47" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B47" s="7">
         <f t="shared" si="0"/>
-        <v>43005</v>
+        <v>42990</v>
       </c>
       <c r="C47" s="11">
-        <v>9.4098841146912946</v>
+        <v>3.686670875798133</v>
       </c>
     </row>
     <row r="48" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B48" s="7">
         <f t="shared" si="0"/>
-        <v>43020</v>
+        <v>43005</v>
       </c>
       <c r="C48" s="11">
-        <v>3.7370042565768635</v>
+        <v>3.9056508250153863</v>
       </c>
     </row>
     <row r="49" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B49" s="7">
         <f t="shared" si="0"/>
-        <v>43035</v>
+        <v>43020</v>
       </c>
       <c r="C49" s="11">
-        <v>3.884872441489903</v>
+        <v>2.6516464586633761</v>
       </c>
     </row>
     <row r="50" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B50" s="7">
         <f t="shared" si="0"/>
-        <v>43050</v>
+        <v>43035</v>
       </c>
       <c r="C50" s="11">
-        <v>6.6806074316484079</v>
+        <v>0.23493298499122958</v>
       </c>
     </row>
     <row r="51" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B51" s="7">
         <f t="shared" si="0"/>
-        <v>43065</v>
+        <v>43050</v>
       </c>
       <c r="C51" s="11">
-        <v>5.2818599662227257</v>
+        <v>2.2695345985447859</v>
       </c>
     </row>
     <row r="52" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B52" s="7">
         <f t="shared" si="0"/>
-        <v>43080</v>
+        <v>43065</v>
       </c>
       <c r="C52" s="11">
-        <v>5.0306173714740856</v>
+        <v>3.2778873891288183</v>
       </c>
     </row>
     <row r="53" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B53" s="7">
         <f t="shared" si="0"/>
-        <v>43095</v>
+        <v>43080</v>
       </c>
       <c r="C53" s="11">
-        <v>5.0769801450758747</v>
+        <v>2.0555395850165294</v>
       </c>
     </row>
     <row r="54" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B54" s="7">
         <f t="shared" si="0"/>
-        <v>43110</v>
+        <v>43095</v>
       </c>
       <c r="C54" s="11">
-        <v>5.5724967934043761</v>
+        <v>1.4067000288659204</v>
       </c>
     </row>
     <row r="55" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B55" s="7">
         <f t="shared" si="0"/>
-        <v>43125</v>
+        <v>43110</v>
       </c>
       <c r="C55" s="11">
-        <v>4.1951096947929578</v>
+        <v>0</v>
       </c>
     </row>
     <row r="56" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B56" s="7">
         <f t="shared" si="0"/>
-        <v>43140</v>
+        <v>43125</v>
       </c>
       <c r="C56" s="11">
-        <v>2.3875447715824505</v>
+        <v>0</v>
       </c>
     </row>
     <row r="57" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B57" s="7">
         <f t="shared" si="0"/>
-        <v>43155</v>
+        <v>43140</v>
       </c>
       <c r="C57" s="11">
-        <v>0</v>
+        <v>1.2844484155122853</v>
       </c>
     </row>
     <row r="58" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B58" s="7">
         <f t="shared" si="0"/>
-        <v>43170</v>
+        <v>43155</v>
       </c>
       <c r="C58" s="11">
-        <v>0</v>
+        <v>1.0690362323696481</v>
       </c>
     </row>
     <row r="59" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B59" s="7">
         <f t="shared" si="0"/>
-        <v>43185</v>
+        <v>43170</v>
       </c>
       <c r="C59" s="11">
-        <v>0.91050756464516125</v>
+        <v>1.6533402775090549</v>
       </c>
     </row>
     <row r="60" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B60" s="7">
         <f t="shared" si="0"/>
-        <v>43200</v>
+        <v>43185</v>
       </c>
       <c r="C60" s="11">
-        <v>14.207884605877252</v>
+        <v>0.84725350097536067</v>
       </c>
     </row>
     <row r="61" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B61" s="7">
         <f t="shared" si="0"/>
-        <v>43215</v>
+        <v>43200</v>
       </c>
       <c r="C61" s="11">
-        <v>20.08437522096602</v>
+        <v>1.5555048134169525</v>
       </c>
     </row>
     <row r="62" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B62" s="7">
         <f t="shared" si="0"/>
-        <v>43230</v>
+        <v>43215</v>
       </c>
       <c r="C62" s="11">
-        <v>37.248532479395813</v>
+        <v>0.12050822542382689</v>
       </c>
     </row>
     <row r="63" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B63" s="7">
         <f t="shared" si="0"/>
-        <v>43245</v>
+        <v>43230</v>
       </c>
       <c r="C63" s="11">
-        <v>93.48921668815882</v>
+        <v>19.24015801632299</v>
       </c>
     </row>
     <row r="64" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B64" s="7">
         <f t="shared" si="0"/>
-        <v>43260</v>
+        <v>43245</v>
       </c>
       <c r="C64" s="11">
-        <v>140.07363864430579</v>
+        <v>44.466884831654596</v>
       </c>
     </row>
     <row r="65" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B65" s="7">
         <f t="shared" si="0"/>
-        <v>43275</v>
+        <v>43260</v>
       </c>
       <c r="C65" s="11">
-        <v>219.48755143385762</v>
+        <v>123.58747827563938</v>
       </c>
     </row>
     <row r="66" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B66" s="7">
         <f t="shared" si="0"/>
-        <v>43290</v>
+        <v>43275</v>
       </c>
       <c r="C66" s="11">
-        <v>257.50144333128566</v>
+        <v>183.35237069607416</v>
       </c>
     </row>
     <row r="67" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B67" s="7">
         <f t="shared" si="0"/>
-        <v>43305</v>
+        <v>43290</v>
       </c>
       <c r="C67" s="11">
-        <v>287.58051598618971</v>
+        <v>203.09191307309914</v>
       </c>
     </row>
     <row r="68" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B68" s="7">
         <f t="shared" si="0"/>
-        <v>43320</v>
+        <v>43305</v>
       </c>
       <c r="C68" s="11">
-        <v>345.71963364839581</v>
+        <v>242.41707847580653</v>
       </c>
     </row>
     <row r="69" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B69" s="7">
         <f t="shared" si="0"/>
-        <v>43335</v>
+        <v>43320</v>
       </c>
       <c r="C69" s="11">
-        <v>418.9177123749684</v>
+        <v>287.21049311362412</v>
       </c>
     </row>
     <row r="70" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B70" s="7">
         <f t="shared" si="0"/>
-        <v>43350</v>
+        <v>43335</v>
       </c>
       <c r="C70" s="11">
-        <v>484.14215321555065</v>
+        <v>327.95712817208903</v>
       </c>
     </row>
     <row r="71" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B71" s="7">
         <f t="shared" si="0"/>
-        <v>43365</v>
+        <v>43350</v>
       </c>
       <c r="C71" s="11">
-        <v>534.1174176641432</v>
+        <v>360.19137260029436</v>
       </c>
     </row>
     <row r="72" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B72" s="7">
         <f t="shared" si="0"/>
-        <v>43380</v>
+        <v>43365</v>
       </c>
       <c r="C72" s="11">
-        <v>596.81580883009633</v>
+        <v>444.69735654145973</v>
       </c>
     </row>
     <row r="73" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B73" s="7">
         <f t="shared" si="0"/>
-        <v>43395</v>
+        <v>43380</v>
       </c>
       <c r="C73" s="11">
-        <v>641.85927527087085</v>
+        <v>565.86072499217551</v>
       </c>
     </row>
     <row r="74" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B74" s="7">
         <f t="shared" si="0"/>
-        <v>43410</v>
+        <v>43395</v>
       </c>
       <c r="C74" s="11">
-        <v>646.78994567192058</v>
+        <v>597.03613590149962</v>
       </c>
     </row>
     <row r="75" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B75" s="7">
         <f t="shared" si="0"/>
-        <v>43425</v>
+        <v>43410</v>
       </c>
       <c r="C75" s="11">
-        <v>677.83475841021925</v>
+        <v>635.73648191409018</v>
       </c>
     </row>
     <row r="76" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B76" s="7">
         <f t="shared" si="0"/>
-        <v>43440</v>
+        <v>43425</v>
       </c>
       <c r="C76" s="11">
-        <v>711.35828379384827</v>
+        <v>686.74653649226775</v>
       </c>
     </row>
     <row r="77" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B77" s="7">
         <f t="shared" si="0"/>
-        <v>43455</v>
+        <v>43440</v>
       </c>
       <c r="C77" s="11">
-        <v>776.4477956452115</v>
+        <v>709.39020323935006</v>
       </c>
     </row>
     <row r="78" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B78" s="7">
         <f t="shared" si="0"/>
-        <v>43470</v>
+        <v>43455</v>
       </c>
       <c r="C78" s="11">
-        <v>837.04067831908981</v>
+        <v>828.84981916110223</v>
       </c>
     </row>
     <row r="79" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B79" s="7">
         <f t="shared" si="0"/>
-        <v>43485</v>
+        <v>43470</v>
       </c>
       <c r="C79" s="11">
-        <v>903.93467461764351</v>
+        <v>832.35594069114131</v>
       </c>
     </row>
     <row r="80" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B80" s="7">
         <f t="shared" si="0"/>
-        <v>43500</v>
+        <v>43485</v>
       </c>
       <c r="C80" s="11">
-        <v>946.65568584893754</v>
+        <v>913.46021052844321</v>
       </c>
     </row>
     <row r="81" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B81" s="7">
         <f t="shared" si="0"/>
-        <v>43515</v>
+        <v>43500</v>
       </c>
       <c r="C81" s="11">
-        <v>1012.7239831227166</v>
+        <v>893.06849684777615</v>
       </c>
     </row>
     <row r="82" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B82" s="7">
         <f t="shared" si="0"/>
-        <v>43530</v>
+        <v>43515</v>
       </c>
       <c r="C82" s="11">
-        <v>1017.3593473935928</v>
+        <v>955.7869342919962</v>
       </c>
     </row>
     <row r="83" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B83" s="7">
         <f t="shared" si="0"/>
-        <v>43545</v>
+        <v>43530</v>
       </c>
       <c r="C83" s="11">
-        <v>1087.4820314195929</v>
+        <v>1010.884074190806</v>
       </c>
     </row>
     <row r="84" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B84" s="7">
         <f t="shared" si="0"/>
-        <v>43560</v>
+        <v>43545</v>
       </c>
       <c r="C84" s="11">
-        <v>1160.9007706132393</v>
+        <v>1027.4566329956604</v>
       </c>
     </row>
     <row r="85" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B85" s="7">
         <f t="shared" si="0"/>
-        <v>43575</v>
+        <v>43560</v>
       </c>
       <c r="C85" s="11">
-        <v>1236.2772736675643</v>
+        <v>1120.4545429487562</v>
       </c>
     </row>
     <row r="86" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B86" s="7">
         <f t="shared" si="0"/>
-        <v>43590</v>
+        <v>43575</v>
       </c>
       <c r="C86" s="11">
-        <v>1243.7606195230567</v>
+        <v>1141.3637680050983</v>
       </c>
     </row>
     <row r="87" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B87" s="7">
         <f t="shared" si="0"/>
-        <v>43605</v>
+        <v>43590</v>
       </c>
       <c r="C87" s="11">
-        <v>1292.5399230650826</v>
+        <v>1140.9472365844526</v>
       </c>
     </row>
     <row r="88" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B88" s="7">
         <f t="shared" si="0"/>
-        <v>43620</v>
+        <v>43605</v>
       </c>
       <c r="C88" s="11">
-        <v>1361.4491862225104</v>
+        <v>1185.8912989073822</v>
       </c>
     </row>
     <row r="89" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B89" s="7">
         <f t="shared" si="0"/>
-        <v>43635</v>
+        <v>43620</v>
       </c>
       <c r="C89" s="11">
-        <v>1414.2334161517551</v>
+        <v>1199.2932153274462</v>
       </c>
     </row>
     <row r="90" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B90" s="7">
         <f t="shared" si="0"/>
-        <v>43650</v>
+        <v>43635</v>
       </c>
       <c r="C90" s="11">
-        <v>1483.1305462166843</v>
+        <v>1240.0842011242521</v>
       </c>
     </row>
     <row r="91" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B91" s="7">
-        <f t="shared" ref="B91:B146" si="1">B90+15</f>
-        <v>43665</v>
+        <f t="shared" si="0"/>
+        <v>43650</v>
       </c>
       <c r="C91" s="11">
-        <v>1541.3556137339494</v>
+        <v>1243.908485019899</v>
       </c>
     </row>
     <row r="92" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B92" s="7">
-        <f t="shared" si="1"/>
-        <v>43680</v>
+        <f t="shared" ref="B92:B147" si="1">B91+15</f>
+        <v>43665</v>
       </c>
       <c r="C92" s="11">
-        <v>1491.5831558670006</v>
+        <v>1288.299242688923</v>
       </c>
     </row>
     <row r="93" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B93" s="7">
         <f t="shared" si="1"/>
-        <v>43695</v>
+        <v>43680</v>
       </c>
       <c r="C93" s="11">
-        <v>1530.1479143460551</v>
+        <v>1224.0748474829259</v>
       </c>
     </row>
     <row r="94" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B94" s="7">
         <f t="shared" si="1"/>
-        <v>43710</v>
+        <v>43695</v>
       </c>
       <c r="C94" s="11">
-        <v>1576.5520669759928</v>
+        <v>1282.2161145644516</v>
       </c>
     </row>
     <row r="95" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B95" s="7">
         <f t="shared" si="1"/>
-        <v>43725</v>
+        <v>43710</v>
       </c>
       <c r="C95" s="11">
-        <v>1602.8396377079198</v>
+        <v>1303.953812402199</v>
       </c>
     </row>
     <row r="96" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B96" s="7">
         <f t="shared" si="1"/>
-        <v>43740</v>
+        <v>43725</v>
       </c>
       <c r="C96" s="11">
-        <v>1621.64031116812</v>
+        <v>1329.3937054089033</v>
       </c>
     </row>
     <row r="97" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B97" s="7">
         <f t="shared" si="1"/>
-        <v>43755</v>
+        <v>43740</v>
       </c>
       <c r="C97" s="11">
-        <v>1666.831403093038</v>
+        <v>1376.4269221127595</v>
       </c>
     </row>
     <row r="98" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B98" s="7">
         <f t="shared" si="1"/>
-        <v>43770</v>
+        <v>43755</v>
       </c>
       <c r="C98" s="11">
-        <v>1572.5012179677531</v>
+        <v>1393.6288149925208</v>
       </c>
     </row>
     <row r="99" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B99" s="7">
         <f t="shared" si="1"/>
-        <v>43785</v>
+        <v>43770</v>
       </c>
       <c r="C99" s="11">
-        <v>1596.3117955128114</v>
+        <v>1325.1575338148511</v>
       </c>
     </row>
     <row r="100" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B100" s="7">
         <f t="shared" si="1"/>
-        <v>43800</v>
+        <v>43785</v>
       </c>
       <c r="C100" s="11">
-        <v>1617.2074911293325</v>
+        <v>1349.8462039338719</v>
       </c>
     </row>
     <row r="101" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B101" s="7">
         <f t="shared" si="1"/>
-        <v>43815</v>
+        <v>43800</v>
       </c>
       <c r="C101" s="11">
-        <v>1639.7155379252808</v>
+        <v>1377.1401349694709</v>
       </c>
     </row>
     <row r="102" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B102" s="7">
         <f t="shared" si="1"/>
-        <v>43830</v>
+        <v>43815</v>
       </c>
       <c r="C102" s="11">
-        <v>1669.0137884368648</v>
+        <v>1403.2077171059793</v>
       </c>
     </row>
     <row r="103" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B103" s="7">
         <f t="shared" si="1"/>
-        <v>43845</v>
+        <v>43830</v>
       </c>
       <c r="C103" s="11">
-        <v>1704.7734763937137</v>
+        <v>1404.1814086812417</v>
       </c>
     </row>
     <row r="104" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B104" s="7">
         <f t="shared" si="1"/>
-        <v>43860</v>
+        <v>43845</v>
       </c>
       <c r="C104" s="11">
-        <v>1721.7231158678751</v>
+        <v>1435.7319990007541</v>
       </c>
     </row>
     <row r="105" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B105" s="7">
         <f t="shared" si="1"/>
-        <v>43875</v>
+        <v>43860</v>
       </c>
       <c r="C105" s="11">
-        <v>1601.3054008782401</v>
+        <v>1464.4938767803901</v>
       </c>
     </row>
     <row r="106" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B106" s="7">
         <f t="shared" si="1"/>
-        <v>43890</v>
+        <v>43875</v>
       </c>
       <c r="C106" s="11">
-        <v>1620.4898270435031</v>
+        <v>1322.213080578701</v>
       </c>
     </row>
     <row r="107" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B107" s="7">
         <f t="shared" si="1"/>
-        <v>43905</v>
+        <v>43890</v>
       </c>
       <c r="C107" s="11">
-        <v>1632.7798332395676</v>
+        <v>1349.9357161289024</v>
       </c>
     </row>
     <row r="108" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B108" s="7">
         <f t="shared" si="1"/>
-        <v>43920</v>
+        <v>43905</v>
       </c>
       <c r="C108" s="11">
-        <v>1649.145077967486</v>
+        <v>1366.3364846764123</v>
       </c>
     </row>
     <row r="109" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B109" s="7">
         <f t="shared" si="1"/>
-        <v>43935</v>
+        <v>43920</v>
       </c>
       <c r="C109" s="11">
-        <v>1671.4495178193251</v>
+        <v>1379.6189207042255</v>
       </c>
     </row>
     <row r="110" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B110" s="7">
         <f t="shared" si="1"/>
-        <v>43950</v>
+        <v>43935</v>
       </c>
       <c r="C110" s="11">
-        <v>1693.9399090570441</v>
+        <v>1428.1226735119735</v>
       </c>
     </row>
     <row r="111" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B111" s="7">
         <f t="shared" si="1"/>
-        <v>43965</v>
+        <v>43950</v>
       </c>
       <c r="C111" s="11">
-        <v>1539.7720457046748</v>
+        <v>1445.7079871938527</v>
       </c>
     </row>
     <row r="112" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B112" s="7">
         <f t="shared" si="1"/>
-        <v>43980</v>
+        <v>43965</v>
       </c>
       <c r="C112" s="11">
-        <v>1558.5115652939269</v>
+        <v>1279.8674474269685</v>
       </c>
     </row>
     <row r="113" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B113" s="7">
         <f t="shared" si="1"/>
-        <v>43995</v>
+        <v>43980</v>
       </c>
       <c r="C113" s="11">
-        <v>1573.2632442473425</v>
+        <v>1287.9056745528653</v>
       </c>
     </row>
     <row r="114" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B114" s="7">
         <f t="shared" si="1"/>
-        <v>44010</v>
+        <v>43995</v>
       </c>
       <c r="C114" s="11">
-        <v>1592.1479094859324</v>
+        <v>1296.6593342879682</v>
       </c>
     </row>
     <row r="115" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B115" s="7">
         <f t="shared" si="1"/>
-        <v>44025</v>
+        <v>44010</v>
       </c>
       <c r="C115" s="11">
-        <v>1599.1224529891049</v>
+        <v>1313.9701291870786</v>
       </c>
     </row>
     <row r="116" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B116" s="7">
         <f t="shared" si="1"/>
-        <v>44040</v>
+        <v>44025</v>
       </c>
       <c r="C116" s="11">
-        <v>1615.786301334294</v>
+        <v>1337.5356523283872</v>
       </c>
     </row>
     <row r="117" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B117" s="7">
         <f t="shared" si="1"/>
-        <v>44055</v>
+        <v>44040</v>
       </c>
       <c r="C117" s="11">
-        <v>1411.0080210997874</v>
+        <v>1348.3240250964293</v>
       </c>
     </row>
     <row r="118" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B118" s="7">
         <f t="shared" si="1"/>
-        <v>44070</v>
+        <v>44055</v>
       </c>
       <c r="C118" s="11">
-        <v>1424.2263678418358</v>
+        <v>1162.8244231391045</v>
       </c>
     </row>
     <row r="119" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B119" s="7">
         <f t="shared" si="1"/>
-        <v>44085</v>
+        <v>44070</v>
       </c>
       <c r="C119" s="11">
-        <v>1435.6297353612122</v>
+        <v>1165.2286023690199</v>
       </c>
     </row>
     <row r="120" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B120" s="7">
         <f t="shared" si="1"/>
-        <v>44100</v>
+        <v>44085</v>
       </c>
       <c r="C120" s="11">
-        <v>1444.5939620911495</v>
+        <v>1166.1137329123385</v>
       </c>
     </row>
     <row r="121" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B121" s="7">
         <f t="shared" si="1"/>
-        <v>44115</v>
+        <v>44100</v>
       </c>
       <c r="C121" s="11">
-        <v>1454.9311122201282</v>
+        <v>1174.9505611698819</v>
       </c>
     </row>
     <row r="122" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B122" s="7">
         <f t="shared" si="1"/>
-        <v>44130</v>
+        <v>44115</v>
       </c>
       <c r="C122" s="11">
-        <v>1473.7640670957662</v>
+        <v>1187.1988058998409</v>
       </c>
     </row>
     <row r="123" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B123" s="7">
         <f t="shared" si="1"/>
-        <v>44145</v>
+        <v>44130</v>
       </c>
       <c r="C123" s="11">
-        <v>1243.1443655145872</v>
+        <v>1198.7151861639536</v>
       </c>
     </row>
     <row r="124" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B124" s="7">
         <f t="shared" si="1"/>
-        <v>44160</v>
+        <v>44145</v>
       </c>
       <c r="C124" s="11">
-        <v>1246.458772956863</v>
+        <v>990.48320610803239</v>
       </c>
     </row>
     <row r="125" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B125" s="7">
         <f t="shared" si="1"/>
-        <v>44175</v>
+        <v>44160</v>
       </c>
       <c r="C125" s="11">
-        <v>1250.1801245204556</v>
+        <v>991.71025151818696</v>
       </c>
     </row>
     <row r="126" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B126" s="7">
         <f t="shared" si="1"/>
-        <v>44190</v>
+        <v>44175</v>
       </c>
       <c r="C126" s="11">
-        <v>1258.4100830775412</v>
+        <v>1004.7614445840968</v>
       </c>
     </row>
     <row r="127" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B127" s="7">
         <f t="shared" si="1"/>
-        <v>44205</v>
+        <v>44190</v>
       </c>
       <c r="C127" s="11">
-        <v>1268.7283489824581</v>
+        <v>1007.2397743879393</v>
       </c>
     </row>
     <row r="128" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B128" s="7">
         <f t="shared" si="1"/>
-        <v>44220</v>
+        <v>44205</v>
       </c>
       <c r="C128" s="11">
-        <v>1281.005602806465</v>
+        <v>1020.5489770455223</v>
       </c>
     </row>
     <row r="129" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B129" s="7">
         <f t="shared" si="1"/>
-        <v>44235</v>
+        <v>44220</v>
       </c>
       <c r="C129" s="11">
-        <v>1029.7735675214969</v>
+        <v>1030.2241902087057</v>
       </c>
     </row>
     <row r="130" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B130" s="7">
         <f t="shared" si="1"/>
-        <v>44250</v>
+        <v>44235</v>
       </c>
       <c r="C130" s="11">
-        <v>1037.1564459421438</v>
+        <v>801.98707976094056</v>
       </c>
     </row>
     <row r="131" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B131" s="7">
         <f t="shared" si="1"/>
-        <v>44265</v>
+        <v>44250</v>
       </c>
       <c r="C131" s="11">
-        <v>1039.5975938678268</v>
+        <v>804.93363602883016</v>
       </c>
     </row>
     <row r="132" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B132" s="7">
         <f t="shared" si="1"/>
-        <v>44280</v>
+        <v>44265</v>
       </c>
       <c r="C132" s="11">
-        <v>1045.1321244180285</v>
+        <v>808.88846947213813</v>
       </c>
     </row>
     <row r="133" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B133" s="7">
         <f t="shared" si="1"/>
-        <v>44295</v>
+        <v>44280</v>
       </c>
       <c r="C133" s="11">
-        <v>1048.2314218646941</v>
+        <v>814.11579808135559</v>
       </c>
     </row>
     <row r="134" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B134" s="7">
         <f t="shared" si="1"/>
-        <v>44310</v>
+        <v>44295</v>
       </c>
       <c r="C134" s="11">
-        <v>1059.2601865500501</v>
+        <v>822.31900902957466</v>
       </c>
     </row>
     <row r="135" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B135" s="7">
         <f t="shared" si="1"/>
-        <v>44325</v>
+        <v>44310</v>
       </c>
       <c r="C135" s="11">
-        <v>784.38358582574813</v>
+        <v>823.41895797462337</v>
       </c>
     </row>
     <row r="136" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B136" s="7">
         <f t="shared" si="1"/>
-        <v>44340</v>
+        <v>44325</v>
       </c>
       <c r="C136" s="11">
-        <v>784.51568238942559</v>
+        <v>577.98199238304335</v>
       </c>
     </row>
     <row r="137" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B137" s="7">
         <f t="shared" si="1"/>
-        <v>44355</v>
+        <v>44340</v>
       </c>
       <c r="C137" s="11">
-        <v>784.59397650783626</v>
+        <v>577.89956794405691</v>
       </c>
     </row>
     <row r="138" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B138" s="7">
         <f t="shared" si="1"/>
-        <v>44370</v>
+        <v>44355</v>
       </c>
       <c r="C138" s="11">
-        <v>785.95759562746662</v>
+        <v>578.26982912862229</v>
       </c>
     </row>
     <row r="139" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B139" s="7">
         <f t="shared" si="1"/>
-        <v>44385</v>
+        <v>44370</v>
       </c>
       <c r="C139" s="11">
-        <v>787.44073155746662</v>
+        <v>578.57441240430626</v>
       </c>
     </row>
     <row r="140" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B140" s="7">
         <f t="shared" si="1"/>
-        <v>44400</v>
+        <v>44385</v>
       </c>
       <c r="C140" s="11">
-        <v>789.2823395128255</v>
+        <v>578.92070392709491</v>
       </c>
     </row>
     <row r="141" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B141" s="7">
         <f t="shared" si="1"/>
-        <v>44415</v>
+        <v>44400</v>
       </c>
       <c r="C141" s="11">
-        <v>485.32972976694367</v>
+        <v>578.84052317282317</v>
       </c>
     </row>
     <row r="142" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B142" s="7">
         <f t="shared" si="1"/>
-        <v>44430</v>
+        <v>44415</v>
       </c>
       <c r="C142" s="11">
-        <v>479.95788106267059</v>
+        <v>306.59207131272933</v>
       </c>
     </row>
     <row r="143" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B143" s="7">
         <f t="shared" si="1"/>
-        <v>44445</v>
+        <v>44430</v>
       </c>
       <c r="C143" s="11">
-        <v>473.81021110626386</v>
+        <v>303.14322533324707</v>
       </c>
     </row>
     <row r="144" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B144" s="7">
         <f t="shared" si="1"/>
-        <v>44460</v>
+        <v>44445</v>
       </c>
       <c r="C144" s="11">
-        <v>469.43690998874439</v>
+        <v>299.3380272572042</v>
       </c>
     </row>
     <row r="145" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B145" s="7">
         <f t="shared" si="1"/>
-        <v>44475</v>
+        <v>44460</v>
       </c>
       <c r="C145" s="11">
-        <v>464.80849303355564</v>
+        <v>293.79157339572407</v>
       </c>
     </row>
     <row r="146" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B146" s="7">
         <f t="shared" si="1"/>
+        <v>44475</v>
+      </c>
+      <c r="C146" s="11">
+        <v>289.7923352371858</v>
+      </c>
+    </row>
+    <row r="147" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B147" s="7">
+        <f t="shared" si="1"/>
         <v>44490</v>
       </c>
-      <c r="C146" s="11">
-        <v>459.815138814985</v>
+      <c r="C147" s="11">
+        <v>285.63079090851278</v>
       </c>
     </row>
   </sheetData>
@@ -2898,7 +2917,7 @@
   <dimension ref="B2:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="B6" sqref="B6:C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2951,7 +2970,7 @@
       </c>
       <c r="C5" s="6" t="str">
         <f>G9</f>
-        <v>ZARSwap.09:10:26-123</v>
+        <v>ZARSwap.21:15:14-6</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>9</v>
@@ -2965,7 +2984,7 @@
         <v>5</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>12</v>
+        <v>35</v>
       </c>
       <c r="F6" s="7">
         <v>42675</v>
@@ -2990,11 +3009,11 @@
     <row r="9" spans="2:7" ht="15" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="str">
         <f>_xll.QSA.CreateHWModelDemo(C2,C3,C4,C5,C6)</f>
-        <v>HWDemo.09:10:26-124</v>
+        <v>HWDemo.21:15:14-7</v>
       </c>
       <c r="G9" s="3" t="str">
         <f>_xll.QSA.CreateDatesAndRatesCurve(G2,F6:F7,G6:G7,G3)</f>
-        <v>ZARSwap.09:10:26-123</v>
+        <v>ZARSwap.21:15:14-6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add JSON serialization. (#53)
* closes #49
* Add new object viewer
* remove IProvidesResultStore.cs.  closes #18. closes #26.
* Add solution level test project.
* Added JSON serialization.
* Removed curve stripping.
* Moving shared data to test helpers.
* Move swaps static constructors into swap factory.
* Add static data files.  Change target version.
* Use SerializableViaName for Excel converters.
</commit_message>
<xml_diff>
--- a/ExcelExamples/BermudanSwaption.xlsx
+++ b/ExcelExamples/BermudanSwaption.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="75" windowWidth="18195" windowHeight="10290" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="72" windowWidth="18192" windowHeight="10296"/>
   </bookViews>
   <sheets>
     <sheet name="Varying exercise dates" sheetId="3" r:id="rId1"/>
     <sheet name="Product&amp;EPE" sheetId="2" r:id="rId2"/>
     <sheet name="Model" sheetId="1" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621" calcMode="manual" calcOnSave="0"/>
+  <calcPr calcId="145621" calcMode="manual" calcCompleted="0" calcOnSave="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="37">
   <si>
     <t>name</t>
   </si>
@@ -54,9 +54,6 @@
     <t>QSA.CreateHWModelDemo</t>
   </si>
   <si>
-    <t>JIBAR3M</t>
-  </si>
-  <si>
     <t>startDate</t>
   </si>
   <si>
@@ -118,6 +115,18 @@
   </si>
   <si>
     <t>Swaption4Ex</t>
+  </si>
+  <si>
+    <t>QSA.GetAvailableResults</t>
+  </si>
+  <si>
+    <t>QSA.GetResults</t>
+  </si>
+  <si>
+    <t>ZAR.JIBAR.3M</t>
+  </si>
+  <si>
+    <t>jibar</t>
   </si>
 </sst>
 </file>
@@ -276,7 +285,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Product&amp;EPE'!$B$25:$B$146</c:f>
+              <c:f>'Product&amp;EPE'!$B$26:$B$147</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm\-yy</c:formatCode>
                 <c:ptCount val="122"/>
@@ -651,7 +660,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Product&amp;EPE'!$C$25:$C$146</c:f>
+              <c:f>'Product&amp;EPE'!$C$26:$C$147</c:f>
               <c:numCache>
                 <c:formatCode>#,##0.00</c:formatCode>
                 <c:ptCount val="122"/>
@@ -659,19 +668,19 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>0.64653070893433173</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>0.49706959177944371</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.27067610339485509</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.58766449057314163</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.33330954272205415</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0</c:v>
@@ -680,346 +689,346 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
+                  <c:v>0.28674479930411617</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.0513201690382024</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10.437653922229206</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>9.1277433160860628</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>6.7256824783779727</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.4382008922410932</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>4.0788148116053273</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>5.4033693396362823</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.170415370404674</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>3.858765170336238</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.92652239358102595</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.2222116728751741</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.76871915779433708</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>3.686670875798133</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>3.9056508250153863</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2.6516464586633761</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.23493298499122958</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2.2695345985447859</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>3.2778873891288183</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2.0555395850165294</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1.4067000288659204</c:v>
+                </c:pt>
+                <c:pt idx="29">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="30">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.16095383044728206</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>2.287870045080393</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0.45330458066640766</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>2.4650942759317331</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>0.3435804514881779</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>6.4394953071166761</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>15.432070455697964</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>12.606054757416631</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>12.457713634014713</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>10.686992351896832</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>12.195249894161828</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>11.294221892745716</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>9.4098841146912946</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>3.7370042565768635</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>3.884872441489903</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>6.6806074316484079</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>5.2818599662227257</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>5.0306173714740856</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>5.0769801450758747</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>5.5724967934043761</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>4.1951096947929578</c:v>
-                </c:pt>
                 <c:pt idx="31">
-                  <c:v>2.3875447715824505</c:v>
+                  <c:v>1.2844484155122853</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0</c:v>
+                  <c:v>1.0690362323696481</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0</c:v>
+                  <c:v>1.6533402775090549</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0.91050756464516125</c:v>
+                  <c:v>0.84725350097536067</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>14.207884605877252</c:v>
+                  <c:v>1.5555048134169525</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>20.08437522096602</c:v>
+                  <c:v>0.12050822542382689</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>37.248532479395813</c:v>
+                  <c:v>19.24015801632299</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>93.48921668815882</c:v>
+                  <c:v>44.466884831654596</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>140.07363864430579</c:v>
+                  <c:v>123.58747827563938</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>219.48755143385762</c:v>
+                  <c:v>183.35237069607416</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>257.50144333128566</c:v>
+                  <c:v>203.09191307309914</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>287.58051598618971</c:v>
+                  <c:v>242.41707847580653</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>345.71963364839581</c:v>
+                  <c:v>287.21049311362412</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>418.9177123749684</c:v>
+                  <c:v>327.95712817208903</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>484.14215321555065</c:v>
+                  <c:v>360.19137260029436</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>534.1174176641432</c:v>
+                  <c:v>444.69735654145973</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>596.81580883009633</c:v>
+                  <c:v>565.86072499217551</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>641.85927527087085</c:v>
+                  <c:v>597.03613590149962</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>646.78994567192058</c:v>
+                  <c:v>635.73648191409018</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>677.83475841021925</c:v>
+                  <c:v>686.74653649226775</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>711.35828379384827</c:v>
+                  <c:v>709.39020323935006</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>776.4477956452115</c:v>
+                  <c:v>828.84981916110223</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>837.04067831908981</c:v>
+                  <c:v>832.35594069114131</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>903.93467461764351</c:v>
+                  <c:v>913.46021052844321</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>946.65568584893754</c:v>
+                  <c:v>893.06849684777615</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>1012.7239831227166</c:v>
+                  <c:v>955.7869342919962</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>1017.3593473935928</c:v>
+                  <c:v>1010.884074190806</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>1087.4820314195929</c:v>
+                  <c:v>1027.4566329956604</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>1160.9007706132393</c:v>
+                  <c:v>1120.4545429487562</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>1236.2772736675643</c:v>
+                  <c:v>1141.3637680050983</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>1243.7606195230567</c:v>
+                  <c:v>1140.9472365844526</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>1292.5399230650826</c:v>
+                  <c:v>1185.8912989073822</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>1361.4491862225104</c:v>
+                  <c:v>1199.2932153274462</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>1414.2334161517551</c:v>
+                  <c:v>1240.0842011242521</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>1483.1305462166843</c:v>
+                  <c:v>1243.908485019899</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>1541.3556137339494</c:v>
+                  <c:v>1288.299242688923</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>1491.5831558670006</c:v>
+                  <c:v>1224.0748474829259</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>1530.1479143460551</c:v>
+                  <c:v>1282.2161145644516</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>1576.5520669759928</c:v>
+                  <c:v>1303.953812402199</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>1602.8396377079198</c:v>
+                  <c:v>1329.3937054089033</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>1621.64031116812</c:v>
+                  <c:v>1376.4269221127595</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>1666.831403093038</c:v>
+                  <c:v>1393.6288149925208</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>1572.5012179677531</c:v>
+                  <c:v>1325.1575338148511</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>1596.3117955128114</c:v>
+                  <c:v>1349.8462039338719</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>1617.2074911293325</c:v>
+                  <c:v>1377.1401349694709</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>1639.7155379252808</c:v>
+                  <c:v>1403.2077171059793</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>1669.0137884368648</c:v>
+                  <c:v>1404.1814086812417</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>1704.7734763937137</c:v>
+                  <c:v>1435.7319990007541</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>1721.7231158678751</c:v>
+                  <c:v>1464.4938767803901</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>1601.3054008782401</c:v>
+                  <c:v>1322.213080578701</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>1620.4898270435031</c:v>
+                  <c:v>1349.9357161289024</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>1632.7798332395676</c:v>
+                  <c:v>1366.3364846764123</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>1649.145077967486</c:v>
+                  <c:v>1379.6189207042255</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>1671.4495178193251</c:v>
+                  <c:v>1428.1226735119735</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>1693.9399090570441</c:v>
+                  <c:v>1445.7079871938527</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>1539.7720457046748</c:v>
+                  <c:v>1279.8674474269685</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>1558.5115652939269</c:v>
+                  <c:v>1287.9056745528653</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>1573.2632442473425</c:v>
+                  <c:v>1296.6593342879682</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>1592.1479094859324</c:v>
+                  <c:v>1313.9701291870786</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>1599.1224529891049</c:v>
+                  <c:v>1337.5356523283872</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>1615.786301334294</c:v>
+                  <c:v>1348.3240250964293</c:v>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>1411.0080210997874</c:v>
+                  <c:v>1162.8244231391045</c:v>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>1424.2263678418358</c:v>
+                  <c:v>1165.2286023690199</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>1435.6297353612122</c:v>
+                  <c:v>1166.1137329123385</c:v>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>1444.5939620911495</c:v>
+                  <c:v>1174.9505611698819</c:v>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>1454.9311122201282</c:v>
+                  <c:v>1187.1988058998409</c:v>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>1473.7640670957662</c:v>
+                  <c:v>1198.7151861639536</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>1243.1443655145872</c:v>
+                  <c:v>990.48320610803239</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>1246.458772956863</c:v>
+                  <c:v>991.71025151818696</c:v>
                 </c:pt>
                 <c:pt idx="100">
-                  <c:v>1250.1801245204556</c:v>
+                  <c:v>1004.7614445840968</c:v>
                 </c:pt>
                 <c:pt idx="101">
-                  <c:v>1258.4100830775412</c:v>
+                  <c:v>1007.2397743879393</c:v>
                 </c:pt>
                 <c:pt idx="102">
-                  <c:v>1268.7283489824581</c:v>
+                  <c:v>1020.5489770455223</c:v>
                 </c:pt>
                 <c:pt idx="103">
-                  <c:v>1281.005602806465</c:v>
+                  <c:v>1030.2241902087057</c:v>
                 </c:pt>
                 <c:pt idx="104">
-                  <c:v>1029.7735675214969</c:v>
+                  <c:v>801.98707976094056</c:v>
                 </c:pt>
                 <c:pt idx="105">
-                  <c:v>1037.1564459421438</c:v>
+                  <c:v>804.93363602883016</c:v>
                 </c:pt>
                 <c:pt idx="106">
-                  <c:v>1039.5975938678268</c:v>
+                  <c:v>808.88846947213813</c:v>
                 </c:pt>
                 <c:pt idx="107">
-                  <c:v>1045.1321244180285</c:v>
+                  <c:v>814.11579808135559</c:v>
                 </c:pt>
                 <c:pt idx="108">
-                  <c:v>1048.2314218646941</c:v>
+                  <c:v>822.31900902957466</c:v>
                 </c:pt>
                 <c:pt idx="109">
-                  <c:v>1059.2601865500501</c:v>
+                  <c:v>823.41895797462337</c:v>
                 </c:pt>
                 <c:pt idx="110">
-                  <c:v>784.38358582574813</c:v>
+                  <c:v>577.98199238304335</c:v>
                 </c:pt>
                 <c:pt idx="111">
-                  <c:v>784.51568238942559</c:v>
+                  <c:v>577.89956794405691</c:v>
                 </c:pt>
                 <c:pt idx="112">
-                  <c:v>784.59397650783626</c:v>
+                  <c:v>578.26982912862229</c:v>
                 </c:pt>
                 <c:pt idx="113">
-                  <c:v>785.95759562746662</c:v>
+                  <c:v>578.57441240430626</c:v>
                 </c:pt>
                 <c:pt idx="114">
-                  <c:v>787.44073155746662</c:v>
+                  <c:v>578.92070392709491</c:v>
                 </c:pt>
                 <c:pt idx="115">
-                  <c:v>789.2823395128255</c:v>
+                  <c:v>578.84052317282317</c:v>
                 </c:pt>
                 <c:pt idx="116">
-                  <c:v>485.32972976694367</c:v>
+                  <c:v>306.59207131272933</c:v>
                 </c:pt>
                 <c:pt idx="117">
-                  <c:v>479.95788106267059</c:v>
+                  <c:v>303.14322533324707</c:v>
                 </c:pt>
                 <c:pt idx="118">
-                  <c:v>473.81021110626386</c:v>
+                  <c:v>299.3380272572042</c:v>
                 </c:pt>
                 <c:pt idx="119">
-                  <c:v>469.43690998874439</c:v>
+                  <c:v>293.79157339572407</c:v>
                 </c:pt>
                 <c:pt idx="120">
-                  <c:v>464.80849303355564</c:v>
+                  <c:v>289.7923352371858</c:v>
                 </c:pt>
                 <c:pt idx="121">
-                  <c:v>459.815138814985</c:v>
+                  <c:v>285.63079090851278</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1036,11 +1045,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="373040256"/>
-        <c:axId val="373045504"/>
+        <c:axId val="201545984"/>
+        <c:axId val="201580544"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="373040256"/>
+        <c:axId val="201545984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1050,14 +1059,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="373045504"/>
+        <c:crossAx val="201580544"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="373045504"/>
+        <c:axId val="201580544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1068,7 +1077,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="373040256"/>
+        <c:crossAx val="201545984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1097,7 +1106,7 @@
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1409,33 +1418,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:E24"/>
+  <dimension ref="B2:E28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C21" sqref="C21:C24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="44.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="33.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="44.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:5" ht="15" x14ac:dyDescent="0.25">
       <c r="E2" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" ht="15" x14ac:dyDescent="0.25">
       <c r="E3" s="7">
         <v>43040</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:5" ht="15" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C4" s="4" t="b">
         <v>0</v>
@@ -1444,9 +1453,9 @@
         <v>43405</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:5" ht="15" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C5" s="7">
         <v>42675</v>
@@ -1455,158 +1464,182 @@
         <v>43770</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:5" ht="15" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>14</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>15</v>
       </c>
       <c r="E6" s="7">
         <v>44136</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:5" ht="15" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C7" s="8">
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:5" ht="15" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C8" s="4" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:5" ht="15" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C9" s="9">
         <v>1000000</v>
       </c>
     </row>
-    <row r="11" spans="2:5" ht="21" x14ac:dyDescent="0.35">
-      <c r="C11" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B12" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="D12" s="3" t="str">
-        <f>_xll.QSA.CreateZARBermudanSwaption(C12,E3,C4,C5,C6,C7,C8,C9)</f>
-        <v>Swaption1Ex.09:10:26-122</v>
-      </c>
-    </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B10" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="C12" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" ht="15" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D13" s="3" t="str">
-        <f>_xll.QSA.CreateZARBermudanSwaption(C13,E3:E4,C4,C5,C6,C7,C8,C9)</f>
-        <v>Swaption2Ex.09:10:26-119</v>
-      </c>
-    </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+        <f ca="1">_xll.QSA.CreateZARBermudanSwaption(C13,$E$3:E3,$C$4,$C$5,$C$6,$C$7,$C$8,$C$9,$C$10)</f>
+        <v>Swaption1Ex.21:17:07-30</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" ht="15" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D14" s="3" t="str">
-        <f>_xll.QSA.CreateZARBermudanSwaption(C14,E3:E5,C4,C5,C6,C7,C8,C9)</f>
-        <v>Swaption3Ex.09:10:26-120</v>
-      </c>
-    </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+        <f ca="1">_xll.QSA.CreateZARBermudanSwaption(C14,$E$3:E4,$C$4,$C$5,$C$6,$C$7,$C$8,$C$9,$C$10)</f>
+        <v>Swaption2Ex.21:17:07-29</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" ht="15" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C15" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D15" s="3" t="str">
+        <f ca="1">_xll.QSA.CreateZARBermudanSwaption(C15,$E$3:E5,$C$4,$C$5,$C$6,$C$7,$C$8,$C$9,$C$10)</f>
+        <v>Swaption3Ex.21:17:07-31</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="B16" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D16" s="3" t="str">
+        <f ca="1">_xll.QSA.CreateZARBermudanSwaption(C16,$E$3:E6,$C$4,$C$5,$C$6,$C$7,$C$8,$C$9,$C$10)</f>
+        <v>Swaption4Ex.21:17:07-32</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B18" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C18" s="10">
+        <f ca="1">Model!F6</f>
+        <v>42675</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B19" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C19" s="6" t="str">
+        <f ca="1">Model!B9</f>
+        <v>HWDemo.21:15:14-7</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B20" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C20" s="4">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" ht="21" x14ac:dyDescent="0.4">
+      <c r="C22" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D15" s="3" t="str">
-        <f>_xll.QSA.CreateZARBermudanSwaption(C15,E3:E6,C4,C5,C6,C7,C8,C9)</f>
-        <v>Swaption4Ex.09:10:26-121</v>
-      </c>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B17" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C17" s="10">
-        <f>Model!F6</f>
-        <v>42675</v>
-      </c>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B18" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C18" s="6" t="str">
-        <f>Model!B9</f>
-        <v>HWDemo.09:10:26-124</v>
-      </c>
-    </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B19" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C19" s="4">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B21" s="3" t="str">
-        <f>_xll.QSA.Value(C12&amp;"Value",D12,$C$17,$C$18,$C$19)</f>
-        <v>Swaption1ExValue.09:10:26-125</v>
-      </c>
-      <c r="C21" s="11">
-        <f>_xll.QSA.GetResults(B21,"value")</f>
-        <v>-9597.2890686645351</v>
-      </c>
-    </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B22" s="3" t="str">
-        <f>_xll.QSA.Value(C13&amp;"Value",D13,$C$17,$C$18,$C$19)</f>
-        <v>Swaption2ExValue.09:10:28-128</v>
-      </c>
-      <c r="C22" s="11">
-        <f>_xll.QSA.GetResults(B22,"value")</f>
-        <v>-11978.432212997121</v>
-      </c>
-    </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B23" s="3" t="str">
-        <f>_xll.QSA.Value(C14&amp;"Value",D14,$C$17,$C$18,$C$19)</f>
-        <v>Swaption3ExValue.09:10:27-127</v>
-      </c>
-      <c r="C23" s="11">
-        <f>_xll.QSA.GetResults(B23,"value")</f>
-        <v>-12965.151497549465</v>
-      </c>
-    </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B24" s="3" t="str">
-        <f>_xll.QSA.Value(C15&amp;"Value",D15,$C$17,$C$18,$C$19)</f>
-        <v>Swaption4ExValue.09:10:27-126</v>
-      </c>
-      <c r="C24" s="11">
-        <f>_xll.QSA.GetResults(B24,"value")</f>
-        <v>-13296.063937555664</v>
+    </row>
+    <row r="23" spans="2:3" ht="21" x14ac:dyDescent="0.4">
+      <c r="C23" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="C24" t="str">
+        <f ca="1">_xll.QSA.GetAvailableResults(B25)</f>
+        <v>value</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B25" s="3" t="str">
+        <f ca="1">_xll.QSA.Value(C13&amp;"Value",D13,$C$18,$C$19,$C$20)</f>
+        <v>Swaption1ExValue.21:17:09-35</v>
+      </c>
+      <c r="C25" s="11">
+        <f ca="1">_xll.QSA.GetResults(B25,"value")</f>
+        <v>-9253.0687187579679</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B26" s="3" t="str">
+        <f ca="1">_xll.QSA.Value(C14&amp;"Value",D14,$C$18,$C$19,$C$20)</f>
+        <v>Swaption2ExValue.21:17:08-34</v>
+      </c>
+      <c r="C26" s="11">
+        <f ca="1">_xll.QSA.GetResults(B26,"value")</f>
+        <v>-11759.643679972569</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B27" s="3" t="str">
+        <f ca="1">_xll.QSA.Value(C15&amp;"Value",D15,$C$18,$C$19,$C$20)</f>
+        <v>Swaption3ExValue.21:17:08-33</v>
+      </c>
+      <c r="C27" s="11">
+        <f ca="1">_xll.QSA.GetResults(B27,"value")</f>
+        <v>-12759.910741854084</v>
+      </c>
+    </row>
+    <row r="28" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B28" s="3" t="str">
+        <f ca="1">_xll.QSA.Value(C16&amp;"Value",D16,$C$18,$C$19,$C$20)</f>
+        <v>Swaption4ExValue.21:17:09-36</v>
+      </c>
+      <c r="C28" s="11">
+        <f ca="1">_xll.QSA.GetResults(B28,"value")</f>
+        <v>-13074.56016657424</v>
       </c>
     </row>
   </sheetData>
@@ -1616,38 +1649,38 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:E146"/>
+  <dimension ref="B2:E147"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F64" sqref="F64"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10:C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="27.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="33.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:5" ht="15" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="2:5" ht="15" x14ac:dyDescent="0.25">
       <c r="E3" s="7">
         <v>43040</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:5" ht="15" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C4" s="4" t="b">
         <v>0</v>
@@ -1656,9 +1689,9 @@
         <v>43405</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:5" ht="15" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C5" s="7">
         <v>42675</v>
@@ -1667,1202 +1700,1210 @@
         <v>43770</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:5" ht="15" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>14</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>15</v>
       </c>
       <c r="E6" s="7">
         <v>44136</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:5" ht="15" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C7" s="8">
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:5" ht="15" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C8" s="4" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:5" ht="15" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C9" s="9">
         <v>1000000</v>
       </c>
     </row>
-    <row r="11" spans="2:5" ht="21" x14ac:dyDescent="0.35">
-      <c r="B11" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B12" s="3" t="str">
-        <f>_xll.QSA.CreateZARBermudanSwaption(C2,E3:E4,C4,C5,C6,C7,C8,C9)</f>
-        <v>BermudanSwaption0001.09:10:26-118</v>
-      </c>
-    </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B15" s="2" t="s">
+    <row r="10" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B10" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="B12" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="B13" s="3" t="str">
+        <f>_xll.QSA.CreateZARBermudanSwaption(C2,E3:E4,C4,C5,C6,C7,C8,C9,C10)</f>
+        <v>BermudanSwaption0001.21:15:14-5</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="B16" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C16" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B17" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" s="6" t="str">
+        <f>B13</f>
+        <v>BermudanSwaption0001.21:15:14-5</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B20" s="2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B16" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C16" s="6" t="str">
-        <f>B12</f>
-        <v>BermudanSwaption0001.09:10:26-118</v>
-      </c>
-    </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B19" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C19" s="10">
+      <c r="C20" s="10">
         <f>Model!F6</f>
         <v>42675</v>
       </c>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B20" s="2" t="s">
+    <row r="21" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B21" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C21" s="6" t="str">
+        <f>Model!B9</f>
+        <v>HWDemo.21:15:14-7</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B22" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C20" s="6" t="str">
-        <f>Model!B9</f>
-        <v>HWDemo.09:10:26-124</v>
-      </c>
-    </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B21" s="2" t="s">
+      <c r="C22" s="4">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" ht="21" x14ac:dyDescent="0.35">
+      <c r="B24" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C21" s="4">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="23" spans="2:3" ht="21" x14ac:dyDescent="0.35">
-      <c r="B23" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B24" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B25" s="7">
-        <f>C19</f>
+    </row>
+    <row r="25" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B25" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B26" s="7">
+        <f>C20</f>
         <v>42675</v>
       </c>
-      <c r="C25" s="11">
-        <f t="array" ref="C25:C146">_xll.QSA.EPE(C16,C19,B25:B146,C20,C21)</f>
+      <c r="C26" s="11">
+        <f t="array" ref="C26:C147">_xll.QSA.EPE(C17,C20,B26:B147,C21,C22)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B26" s="7">
-        <f>B25+15</f>
+    <row r="27" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B27" s="7">
+        <f>B26+15</f>
         <v>42690</v>
       </c>
-      <c r="C26" s="11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B27" s="7">
-        <f t="shared" ref="B27:B90" si="0">B26+15</f>
+      <c r="C27" s="11">
+        <v>0.64653070893433173</v>
+      </c>
+    </row>
+    <row r="28" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B28" s="7">
+        <f t="shared" ref="B28:B91" si="0">B27+15</f>
         <v>42705</v>
-      </c>
-      <c r="C27" s="11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B28" s="7">
-        <f t="shared" si="0"/>
-        <v>42720</v>
       </c>
       <c r="C28" s="11">
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B29" s="7">
         <f t="shared" si="0"/>
+        <v>42720</v>
+      </c>
+      <c r="C29" s="11">
+        <v>0.49706959177944371</v>
+      </c>
+    </row>
+    <row r="30" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B30" s="7">
+        <f t="shared" si="0"/>
         <v>42735</v>
       </c>
-      <c r="C29" s="11">
-        <v>0.58766449057314163</v>
-      </c>
-    </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B30" s="7">
+      <c r="C30" s="11">
+        <v>0.27067610339485509</v>
+      </c>
+    </row>
+    <row r="31" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B31" s="7">
         <f t="shared" si="0"/>
         <v>42750</v>
-      </c>
-      <c r="C30" s="11">
-        <v>0.33330954272205415</v>
-      </c>
-    </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B31" s="7">
-        <f t="shared" si="0"/>
-        <v>42765</v>
       </c>
       <c r="C31" s="11">
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B32" s="7">
         <f t="shared" si="0"/>
-        <v>42780</v>
+        <v>42765</v>
       </c>
       <c r="C32" s="11">
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B33" s="7">
         <f t="shared" si="0"/>
-        <v>42795</v>
+        <v>42780</v>
       </c>
       <c r="C33" s="11">
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B34" s="7">
         <f t="shared" si="0"/>
+        <v>42795</v>
+      </c>
+      <c r="C34" s="11">
+        <v>0.28674479930411617</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B35" s="7">
+        <f t="shared" si="0"/>
         <v>42810</v>
       </c>
-      <c r="C34" s="11">
+      <c r="C35" s="11">
+        <v>1.0513201690382024</v>
+      </c>
+    </row>
+    <row r="36" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B36" s="7">
+        <f t="shared" si="0"/>
+        <v>42825</v>
+      </c>
+      <c r="C36" s="11">
+        <v>10.437653922229206</v>
+      </c>
+    </row>
+    <row r="37" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B37" s="7">
+        <f t="shared" si="0"/>
+        <v>42840</v>
+      </c>
+      <c r="C37" s="11">
+        <v>9.1277433160860628</v>
+      </c>
+    </row>
+    <row r="38" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B38" s="7">
+        <f t="shared" si="0"/>
+        <v>42855</v>
+      </c>
+      <c r="C38" s="11">
+        <v>6.7256824783779727</v>
+      </c>
+    </row>
+    <row r="39" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B39" s="7">
+        <f t="shared" si="0"/>
+        <v>42870</v>
+      </c>
+      <c r="C39" s="11">
+        <v>1.4382008922410932</v>
+      </c>
+    </row>
+    <row r="40" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B40" s="7">
+        <f t="shared" si="0"/>
+        <v>42885</v>
+      </c>
+      <c r="C40" s="11">
+        <v>4.0788148116053273</v>
+      </c>
+    </row>
+    <row r="41" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B41" s="7">
+        <f t="shared" si="0"/>
+        <v>42900</v>
+      </c>
+      <c r="C41" s="11">
+        <v>5.4033693396362823</v>
+      </c>
+    </row>
+    <row r="42" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B42" s="7">
+        <f t="shared" si="0"/>
+        <v>42915</v>
+      </c>
+      <c r="C42" s="11">
+        <v>1.170415370404674</v>
+      </c>
+    </row>
+    <row r="43" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B43" s="7">
+        <f t="shared" si="0"/>
+        <v>42930</v>
+      </c>
+      <c r="C43" s="11">
+        <v>3.858765170336238</v>
+      </c>
+    </row>
+    <row r="44" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B44" s="7">
+        <f t="shared" si="0"/>
+        <v>42945</v>
+      </c>
+      <c r="C44" s="11">
+        <v>0.92652239358102595</v>
+      </c>
+    </row>
+    <row r="45" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B45" s="7">
+        <f t="shared" si="0"/>
+        <v>42960</v>
+      </c>
+      <c r="C45" s="11">
+        <v>0.2222116728751741</v>
+      </c>
+    </row>
+    <row r="46" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B46" s="7">
+        <f t="shared" si="0"/>
+        <v>42975</v>
+      </c>
+      <c r="C46" s="11">
+        <v>0.76871915779433708</v>
+      </c>
+    </row>
+    <row r="47" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B47" s="7">
+        <f t="shared" si="0"/>
+        <v>42990</v>
+      </c>
+      <c r="C47" s="11">
+        <v>3.686670875798133</v>
+      </c>
+    </row>
+    <row r="48" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B48" s="7">
+        <f t="shared" si="0"/>
+        <v>43005</v>
+      </c>
+      <c r="C48" s="11">
+        <v>3.9056508250153863</v>
+      </c>
+    </row>
+    <row r="49" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B49" s="7">
+        <f t="shared" si="0"/>
+        <v>43020</v>
+      </c>
+      <c r="C49" s="11">
+        <v>2.6516464586633761</v>
+      </c>
+    </row>
+    <row r="50" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B50" s="7">
+        <f t="shared" si="0"/>
+        <v>43035</v>
+      </c>
+      <c r="C50" s="11">
+        <v>0.23493298499122958</v>
+      </c>
+    </row>
+    <row r="51" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B51" s="7">
+        <f t="shared" si="0"/>
+        <v>43050</v>
+      </c>
+      <c r="C51" s="11">
+        <v>2.2695345985447859</v>
+      </c>
+    </row>
+    <row r="52" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B52" s="7">
+        <f t="shared" si="0"/>
+        <v>43065</v>
+      </c>
+      <c r="C52" s="11">
+        <v>3.2778873891288183</v>
+      </c>
+    </row>
+    <row r="53" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B53" s="7">
+        <f t="shared" si="0"/>
+        <v>43080</v>
+      </c>
+      <c r="C53" s="11">
+        <v>2.0555395850165294</v>
+      </c>
+    </row>
+    <row r="54" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B54" s="7">
+        <f t="shared" si="0"/>
+        <v>43095</v>
+      </c>
+      <c r="C54" s="11">
+        <v>1.4067000288659204</v>
+      </c>
+    </row>
+    <row r="55" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B55" s="7">
+        <f t="shared" si="0"/>
+        <v>43110</v>
+      </c>
+      <c r="C55" s="11">
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B35" s="7">
-        <f t="shared" si="0"/>
-        <v>42825</v>
-      </c>
-      <c r="C35" s="11">
-        <v>0.16095383044728206</v>
-      </c>
-    </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B36" s="7">
-        <f t="shared" si="0"/>
-        <v>42840</v>
-      </c>
-      <c r="C36" s="11">
-        <v>2.287870045080393</v>
-      </c>
-    </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B37" s="7">
-        <f t="shared" si="0"/>
-        <v>42855</v>
-      </c>
-      <c r="C37" s="11">
-        <v>0.45330458066640766</v>
-      </c>
-    </row>
-    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B38" s="7">
-        <f t="shared" si="0"/>
-        <v>42870</v>
-      </c>
-      <c r="C38" s="11">
-        <v>2.4650942759317331</v>
-      </c>
-    </row>
-    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B39" s="7">
-        <f t="shared" si="0"/>
-        <v>42885</v>
-      </c>
-      <c r="C39" s="11">
-        <v>0.3435804514881779</v>
-      </c>
-    </row>
-    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B40" s="7">
-        <f t="shared" si="0"/>
-        <v>42900</v>
-      </c>
-      <c r="C40" s="11">
-        <v>6.4394953071166761</v>
-      </c>
-    </row>
-    <row r="41" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B41" s="7">
-        <f t="shared" si="0"/>
-        <v>42915</v>
-      </c>
-      <c r="C41" s="11">
-        <v>15.432070455697964</v>
-      </c>
-    </row>
-    <row r="42" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B42" s="7">
-        <f t="shared" si="0"/>
-        <v>42930</v>
-      </c>
-      <c r="C42" s="11">
-        <v>12.606054757416631</v>
-      </c>
-    </row>
-    <row r="43" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B43" s="7">
-        <f t="shared" si="0"/>
-        <v>42945</v>
-      </c>
-      <c r="C43" s="11">
-        <v>12.457713634014713</v>
-      </c>
-    </row>
-    <row r="44" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B44" s="7">
-        <f t="shared" si="0"/>
-        <v>42960</v>
-      </c>
-      <c r="C44" s="11">
-        <v>10.686992351896832</v>
-      </c>
-    </row>
-    <row r="45" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B45" s="7">
-        <f t="shared" si="0"/>
-        <v>42975</v>
-      </c>
-      <c r="C45" s="11">
-        <v>12.195249894161828</v>
-      </c>
-    </row>
-    <row r="46" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B46" s="7">
-        <f t="shared" si="0"/>
-        <v>42990</v>
-      </c>
-      <c r="C46" s="11">
-        <v>11.294221892745716</v>
-      </c>
-    </row>
-    <row r="47" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B47" s="7">
-        <f t="shared" si="0"/>
-        <v>43005</v>
-      </c>
-      <c r="C47" s="11">
-        <v>9.4098841146912946</v>
-      </c>
-    </row>
-    <row r="48" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B48" s="7">
-        <f t="shared" si="0"/>
-        <v>43020</v>
-      </c>
-      <c r="C48" s="11">
-        <v>3.7370042565768635</v>
-      </c>
-    </row>
-    <row r="49" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B49" s="7">
-        <f t="shared" si="0"/>
-        <v>43035</v>
-      </c>
-      <c r="C49" s="11">
-        <v>3.884872441489903</v>
-      </c>
-    </row>
-    <row r="50" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B50" s="7">
-        <f t="shared" si="0"/>
-        <v>43050</v>
-      </c>
-      <c r="C50" s="11">
-        <v>6.6806074316484079</v>
-      </c>
-    </row>
-    <row r="51" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B51" s="7">
-        <f t="shared" si="0"/>
-        <v>43065</v>
-      </c>
-      <c r="C51" s="11">
-        <v>5.2818599662227257</v>
-      </c>
-    </row>
-    <row r="52" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B52" s="7">
-        <f t="shared" si="0"/>
-        <v>43080</v>
-      </c>
-      <c r="C52" s="11">
-        <v>5.0306173714740856</v>
-      </c>
-    </row>
-    <row r="53" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B53" s="7">
-        <f t="shared" si="0"/>
-        <v>43095</v>
-      </c>
-      <c r="C53" s="11">
-        <v>5.0769801450758747</v>
-      </c>
-    </row>
-    <row r="54" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B54" s="7">
-        <f t="shared" si="0"/>
-        <v>43110</v>
-      </c>
-      <c r="C54" s="11">
-        <v>5.5724967934043761</v>
-      </c>
-    </row>
-    <row r="55" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B55" s="7">
+    <row r="56" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B56" s="7">
         <f t="shared" si="0"/>
         <v>43125</v>
       </c>
-      <c r="C55" s="11">
-        <v>4.1951096947929578</v>
-      </c>
-    </row>
-    <row r="56" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B56" s="7">
+      <c r="C56" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B57" s="7">
         <f t="shared" si="0"/>
         <v>43140</v>
       </c>
-      <c r="C56" s="11">
-        <v>2.3875447715824505</v>
-      </c>
-    </row>
-    <row r="57" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B57" s="7">
+      <c r="C57" s="11">
+        <v>1.2844484155122853</v>
+      </c>
+    </row>
+    <row r="58" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B58" s="7">
         <f t="shared" si="0"/>
         <v>43155</v>
       </c>
-      <c r="C57" s="11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B58" s="7">
+      <c r="C58" s="11">
+        <v>1.0690362323696481</v>
+      </c>
+    </row>
+    <row r="59" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B59" s="7">
         <f t="shared" si="0"/>
         <v>43170</v>
       </c>
-      <c r="C58" s="11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B59" s="7">
+      <c r="C59" s="11">
+        <v>1.6533402775090549</v>
+      </c>
+    </row>
+    <row r="60" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B60" s="7">
         <f t="shared" si="0"/>
         <v>43185</v>
       </c>
-      <c r="C59" s="11">
-        <v>0.91050756464516125</v>
-      </c>
-    </row>
-    <row r="60" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B60" s="7">
+      <c r="C60" s="11">
+        <v>0.84725350097536067</v>
+      </c>
+    </row>
+    <row r="61" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B61" s="7">
         <f t="shared" si="0"/>
         <v>43200</v>
       </c>
-      <c r="C60" s="11">
-        <v>14.207884605877252</v>
-      </c>
-    </row>
-    <row r="61" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B61" s="7">
+      <c r="C61" s="11">
+        <v>1.5555048134169525</v>
+      </c>
+    </row>
+    <row r="62" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B62" s="7">
         <f t="shared" si="0"/>
         <v>43215</v>
       </c>
-      <c r="C61" s="11">
-        <v>20.08437522096602</v>
-      </c>
-    </row>
-    <row r="62" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B62" s="7">
+      <c r="C62" s="11">
+        <v>0.12050822542382689</v>
+      </c>
+    </row>
+    <row r="63" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B63" s="7">
         <f t="shared" si="0"/>
         <v>43230</v>
       </c>
-      <c r="C62" s="11">
-        <v>37.248532479395813</v>
-      </c>
-    </row>
-    <row r="63" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B63" s="7">
+      <c r="C63" s="11">
+        <v>19.24015801632299</v>
+      </c>
+    </row>
+    <row r="64" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B64" s="7">
         <f t="shared" si="0"/>
         <v>43245</v>
       </c>
-      <c r="C63" s="11">
-        <v>93.48921668815882</v>
-      </c>
-    </row>
-    <row r="64" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B64" s="7">
+      <c r="C64" s="11">
+        <v>44.466884831654596</v>
+      </c>
+    </row>
+    <row r="65" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B65" s="7">
         <f t="shared" si="0"/>
         <v>43260</v>
       </c>
-      <c r="C64" s="11">
-        <v>140.07363864430579</v>
-      </c>
-    </row>
-    <row r="65" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B65" s="7">
+      <c r="C65" s="11">
+        <v>123.58747827563938</v>
+      </c>
+    </row>
+    <row r="66" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B66" s="7">
         <f t="shared" si="0"/>
         <v>43275</v>
       </c>
-      <c r="C65" s="11">
-        <v>219.48755143385762</v>
-      </c>
-    </row>
-    <row r="66" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B66" s="7">
+      <c r="C66" s="11">
+        <v>183.35237069607416</v>
+      </c>
+    </row>
+    <row r="67" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B67" s="7">
         <f t="shared" si="0"/>
         <v>43290</v>
       </c>
-      <c r="C66" s="11">
-        <v>257.50144333128566</v>
-      </c>
-    </row>
-    <row r="67" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B67" s="7">
+      <c r="C67" s="11">
+        <v>203.09191307309914</v>
+      </c>
+    </row>
+    <row r="68" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B68" s="7">
         <f t="shared" si="0"/>
         <v>43305</v>
       </c>
-      <c r="C67" s="11">
-        <v>287.58051598618971</v>
-      </c>
-    </row>
-    <row r="68" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B68" s="7">
+      <c r="C68" s="11">
+        <v>242.41707847580653</v>
+      </c>
+    </row>
+    <row r="69" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B69" s="7">
         <f t="shared" si="0"/>
         <v>43320</v>
       </c>
-      <c r="C68" s="11">
-        <v>345.71963364839581</v>
-      </c>
-    </row>
-    <row r="69" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B69" s="7">
+      <c r="C69" s="11">
+        <v>287.21049311362412</v>
+      </c>
+    </row>
+    <row r="70" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B70" s="7">
         <f t="shared" si="0"/>
         <v>43335</v>
       </c>
-      <c r="C69" s="11">
-        <v>418.9177123749684</v>
-      </c>
-    </row>
-    <row r="70" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B70" s="7">
+      <c r="C70" s="11">
+        <v>327.95712817208903</v>
+      </c>
+    </row>
+    <row r="71" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B71" s="7">
         <f t="shared" si="0"/>
         <v>43350</v>
       </c>
-      <c r="C70" s="11">
-        <v>484.14215321555065</v>
-      </c>
-    </row>
-    <row r="71" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B71" s="7">
+      <c r="C71" s="11">
+        <v>360.19137260029436</v>
+      </c>
+    </row>
+    <row r="72" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B72" s="7">
         <f t="shared" si="0"/>
         <v>43365</v>
       </c>
-      <c r="C71" s="11">
-        <v>534.1174176641432</v>
-      </c>
-    </row>
-    <row r="72" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B72" s="7">
+      <c r="C72" s="11">
+        <v>444.69735654145973</v>
+      </c>
+    </row>
+    <row r="73" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B73" s="7">
         <f t="shared" si="0"/>
         <v>43380</v>
       </c>
-      <c r="C72" s="11">
-        <v>596.81580883009633</v>
-      </c>
-    </row>
-    <row r="73" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B73" s="7">
+      <c r="C73" s="11">
+        <v>565.86072499217551</v>
+      </c>
+    </row>
+    <row r="74" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B74" s="7">
         <f t="shared" si="0"/>
         <v>43395</v>
       </c>
-      <c r="C73" s="11">
-        <v>641.85927527087085</v>
-      </c>
-    </row>
-    <row r="74" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B74" s="7">
+      <c r="C74" s="11">
+        <v>597.03613590149962</v>
+      </c>
+    </row>
+    <row r="75" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B75" s="7">
         <f t="shared" si="0"/>
         <v>43410</v>
       </c>
-      <c r="C74" s="11">
-        <v>646.78994567192058</v>
-      </c>
-    </row>
-    <row r="75" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B75" s="7">
+      <c r="C75" s="11">
+        <v>635.73648191409018</v>
+      </c>
+    </row>
+    <row r="76" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B76" s="7">
         <f t="shared" si="0"/>
         <v>43425</v>
       </c>
-      <c r="C75" s="11">
-        <v>677.83475841021925</v>
-      </c>
-    </row>
-    <row r="76" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B76" s="7">
+      <c r="C76" s="11">
+        <v>686.74653649226775</v>
+      </c>
+    </row>
+    <row r="77" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B77" s="7">
         <f t="shared" si="0"/>
         <v>43440</v>
       </c>
-      <c r="C76" s="11">
-        <v>711.35828379384827</v>
-      </c>
-    </row>
-    <row r="77" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B77" s="7">
+      <c r="C77" s="11">
+        <v>709.39020323935006</v>
+      </c>
+    </row>
+    <row r="78" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B78" s="7">
         <f t="shared" si="0"/>
         <v>43455</v>
       </c>
-      <c r="C77" s="11">
-        <v>776.4477956452115</v>
-      </c>
-    </row>
-    <row r="78" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B78" s="7">
+      <c r="C78" s="11">
+        <v>828.84981916110223</v>
+      </c>
+    </row>
+    <row r="79" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B79" s="7">
         <f t="shared" si="0"/>
         <v>43470</v>
       </c>
-      <c r="C78" s="11">
-        <v>837.04067831908981</v>
-      </c>
-    </row>
-    <row r="79" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B79" s="7">
+      <c r="C79" s="11">
+        <v>832.35594069114131</v>
+      </c>
+    </row>
+    <row r="80" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B80" s="7">
         <f t="shared" si="0"/>
         <v>43485</v>
       </c>
-      <c r="C79" s="11">
-        <v>903.93467461764351</v>
-      </c>
-    </row>
-    <row r="80" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B80" s="7">
+      <c r="C80" s="11">
+        <v>913.46021052844321</v>
+      </c>
+    </row>
+    <row r="81" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B81" s="7">
         <f t="shared" si="0"/>
         <v>43500</v>
       </c>
-      <c r="C80" s="11">
-        <v>946.65568584893754</v>
-      </c>
-    </row>
-    <row r="81" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B81" s="7">
+      <c r="C81" s="11">
+        <v>893.06849684777615</v>
+      </c>
+    </row>
+    <row r="82" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B82" s="7">
         <f t="shared" si="0"/>
         <v>43515</v>
       </c>
-      <c r="C81" s="11">
-        <v>1012.7239831227166</v>
-      </c>
-    </row>
-    <row r="82" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B82" s="7">
+      <c r="C82" s="11">
+        <v>955.7869342919962</v>
+      </c>
+    </row>
+    <row r="83" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B83" s="7">
         <f t="shared" si="0"/>
         <v>43530</v>
       </c>
-      <c r="C82" s="11">
-        <v>1017.3593473935928</v>
-      </c>
-    </row>
-    <row r="83" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B83" s="7">
+      <c r="C83" s="11">
+        <v>1010.884074190806</v>
+      </c>
+    </row>
+    <row r="84" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B84" s="7">
         <f t="shared" si="0"/>
         <v>43545</v>
       </c>
-      <c r="C83" s="11">
-        <v>1087.4820314195929</v>
-      </c>
-    </row>
-    <row r="84" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B84" s="7">
+      <c r="C84" s="11">
+        <v>1027.4566329956604</v>
+      </c>
+    </row>
+    <row r="85" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B85" s="7">
         <f t="shared" si="0"/>
         <v>43560</v>
       </c>
-      <c r="C84" s="11">
-        <v>1160.9007706132393</v>
-      </c>
-    </row>
-    <row r="85" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B85" s="7">
+      <c r="C85" s="11">
+        <v>1120.4545429487562</v>
+      </c>
+    </row>
+    <row r="86" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B86" s="7">
         <f t="shared" si="0"/>
         <v>43575</v>
       </c>
-      <c r="C85" s="11">
-        <v>1236.2772736675643</v>
-      </c>
-    </row>
-    <row r="86" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B86" s="7">
+      <c r="C86" s="11">
+        <v>1141.3637680050983</v>
+      </c>
+    </row>
+    <row r="87" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B87" s="7">
         <f t="shared" si="0"/>
         <v>43590</v>
       </c>
-      <c r="C86" s="11">
-        <v>1243.7606195230567</v>
-      </c>
-    </row>
-    <row r="87" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B87" s="7">
+      <c r="C87" s="11">
+        <v>1140.9472365844526</v>
+      </c>
+    </row>
+    <row r="88" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B88" s="7">
         <f t="shared" si="0"/>
         <v>43605</v>
       </c>
-      <c r="C87" s="11">
-        <v>1292.5399230650826</v>
-      </c>
-    </row>
-    <row r="88" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B88" s="7">
+      <c r="C88" s="11">
+        <v>1185.8912989073822</v>
+      </c>
+    </row>
+    <row r="89" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B89" s="7">
         <f t="shared" si="0"/>
         <v>43620</v>
       </c>
-      <c r="C88" s="11">
-        <v>1361.4491862225104</v>
-      </c>
-    </row>
-    <row r="89" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B89" s="7">
+      <c r="C89" s="11">
+        <v>1199.2932153274462</v>
+      </c>
+    </row>
+    <row r="90" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B90" s="7">
         <f t="shared" si="0"/>
         <v>43635</v>
       </c>
-      <c r="C89" s="11">
-        <v>1414.2334161517551</v>
-      </c>
-    </row>
-    <row r="90" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B90" s="7">
+      <c r="C90" s="11">
+        <v>1240.0842011242521</v>
+      </c>
+    </row>
+    <row r="91" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B91" s="7">
         <f t="shared" si="0"/>
         <v>43650</v>
       </c>
-      <c r="C90" s="11">
-        <v>1483.1305462166843</v>
-      </c>
-    </row>
-    <row r="91" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B91" s="7">
-        <f t="shared" ref="B91:B146" si="1">B90+15</f>
+      <c r="C91" s="11">
+        <v>1243.908485019899</v>
+      </c>
+    </row>
+    <row r="92" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B92" s="7">
+        <f t="shared" ref="B92:B147" si="1">B91+15</f>
         <v>43665</v>
       </c>
-      <c r="C91" s="11">
-        <v>1541.3556137339494</v>
-      </c>
-    </row>
-    <row r="92" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B92" s="7">
+      <c r="C92" s="11">
+        <v>1288.299242688923</v>
+      </c>
+    </row>
+    <row r="93" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B93" s="7">
         <f t="shared" si="1"/>
         <v>43680</v>
       </c>
-      <c r="C92" s="11">
-        <v>1491.5831558670006</v>
-      </c>
-    </row>
-    <row r="93" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B93" s="7">
+      <c r="C93" s="11">
+        <v>1224.0748474829259</v>
+      </c>
+    </row>
+    <row r="94" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B94" s="7">
         <f t="shared" si="1"/>
         <v>43695</v>
       </c>
-      <c r="C93" s="11">
-        <v>1530.1479143460551</v>
-      </c>
-    </row>
-    <row r="94" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B94" s="7">
+      <c r="C94" s="11">
+        <v>1282.2161145644516</v>
+      </c>
+    </row>
+    <row r="95" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B95" s="7">
         <f t="shared" si="1"/>
         <v>43710</v>
       </c>
-      <c r="C94" s="11">
-        <v>1576.5520669759928</v>
-      </c>
-    </row>
-    <row r="95" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B95" s="7">
+      <c r="C95" s="11">
+        <v>1303.953812402199</v>
+      </c>
+    </row>
+    <row r="96" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B96" s="7">
         <f t="shared" si="1"/>
         <v>43725</v>
       </c>
-      <c r="C95" s="11">
-        <v>1602.8396377079198</v>
-      </c>
-    </row>
-    <row r="96" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B96" s="7">
+      <c r="C96" s="11">
+        <v>1329.3937054089033</v>
+      </c>
+    </row>
+    <row r="97" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B97" s="7">
         <f t="shared" si="1"/>
         <v>43740</v>
       </c>
-      <c r="C96" s="11">
-        <v>1621.64031116812</v>
-      </c>
-    </row>
-    <row r="97" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B97" s="7">
+      <c r="C97" s="11">
+        <v>1376.4269221127595</v>
+      </c>
+    </row>
+    <row r="98" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B98" s="7">
         <f t="shared" si="1"/>
         <v>43755</v>
       </c>
-      <c r="C97" s="11">
-        <v>1666.831403093038</v>
-      </c>
-    </row>
-    <row r="98" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B98" s="7">
+      <c r="C98" s="11">
+        <v>1393.6288149925208</v>
+      </c>
+    </row>
+    <row r="99" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B99" s="7">
         <f t="shared" si="1"/>
         <v>43770</v>
       </c>
-      <c r="C98" s="11">
-        <v>1572.5012179677531</v>
-      </c>
-    </row>
-    <row r="99" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B99" s="7">
+      <c r="C99" s="11">
+        <v>1325.1575338148511</v>
+      </c>
+    </row>
+    <row r="100" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B100" s="7">
         <f t="shared" si="1"/>
         <v>43785</v>
       </c>
-      <c r="C99" s="11">
-        <v>1596.3117955128114</v>
-      </c>
-    </row>
-    <row r="100" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B100" s="7">
+      <c r="C100" s="11">
+        <v>1349.8462039338719</v>
+      </c>
+    </row>
+    <row r="101" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B101" s="7">
         <f t="shared" si="1"/>
         <v>43800</v>
       </c>
-      <c r="C100" s="11">
-        <v>1617.2074911293325</v>
-      </c>
-    </row>
-    <row r="101" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B101" s="7">
+      <c r="C101" s="11">
+        <v>1377.1401349694709</v>
+      </c>
+    </row>
+    <row r="102" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B102" s="7">
         <f t="shared" si="1"/>
         <v>43815</v>
       </c>
-      <c r="C101" s="11">
-        <v>1639.7155379252808</v>
-      </c>
-    </row>
-    <row r="102" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B102" s="7">
+      <c r="C102" s="11">
+        <v>1403.2077171059793</v>
+      </c>
+    </row>
+    <row r="103" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B103" s="7">
         <f t="shared" si="1"/>
         <v>43830</v>
       </c>
-      <c r="C102" s="11">
-        <v>1669.0137884368648</v>
-      </c>
-    </row>
-    <row r="103" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B103" s="7">
+      <c r="C103" s="11">
+        <v>1404.1814086812417</v>
+      </c>
+    </row>
+    <row r="104" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B104" s="7">
         <f t="shared" si="1"/>
         <v>43845</v>
       </c>
-      <c r="C103" s="11">
-        <v>1704.7734763937137</v>
-      </c>
-    </row>
-    <row r="104" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B104" s="7">
+      <c r="C104" s="11">
+        <v>1435.7319990007541</v>
+      </c>
+    </row>
+    <row r="105" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B105" s="7">
         <f t="shared" si="1"/>
         <v>43860</v>
       </c>
-      <c r="C104" s="11">
-        <v>1721.7231158678751</v>
-      </c>
-    </row>
-    <row r="105" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B105" s="7">
+      <c r="C105" s="11">
+        <v>1464.4938767803901</v>
+      </c>
+    </row>
+    <row r="106" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B106" s="7">
         <f t="shared" si="1"/>
         <v>43875</v>
       </c>
-      <c r="C105" s="11">
-        <v>1601.3054008782401</v>
-      </c>
-    </row>
-    <row r="106" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B106" s="7">
+      <c r="C106" s="11">
+        <v>1322.213080578701</v>
+      </c>
+    </row>
+    <row r="107" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B107" s="7">
         <f t="shared" si="1"/>
         <v>43890</v>
       </c>
-      <c r="C106" s="11">
-        <v>1620.4898270435031</v>
-      </c>
-    </row>
-    <row r="107" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B107" s="7">
+      <c r="C107" s="11">
+        <v>1349.9357161289024</v>
+      </c>
+    </row>
+    <row r="108" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B108" s="7">
         <f t="shared" si="1"/>
         <v>43905</v>
       </c>
-      <c r="C107" s="11">
-        <v>1632.7798332395676</v>
-      </c>
-    </row>
-    <row r="108" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B108" s="7">
+      <c r="C108" s="11">
+        <v>1366.3364846764123</v>
+      </c>
+    </row>
+    <row r="109" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B109" s="7">
         <f t="shared" si="1"/>
         <v>43920</v>
       </c>
-      <c r="C108" s="11">
-        <v>1649.145077967486</v>
-      </c>
-    </row>
-    <row r="109" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B109" s="7">
+      <c r="C109" s="11">
+        <v>1379.6189207042255</v>
+      </c>
+    </row>
+    <row r="110" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B110" s="7">
         <f t="shared" si="1"/>
         <v>43935</v>
       </c>
-      <c r="C109" s="11">
-        <v>1671.4495178193251</v>
-      </c>
-    </row>
-    <row r="110" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B110" s="7">
+      <c r="C110" s="11">
+        <v>1428.1226735119735</v>
+      </c>
+    </row>
+    <row r="111" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B111" s="7">
         <f t="shared" si="1"/>
         <v>43950</v>
       </c>
-      <c r="C110" s="11">
-        <v>1693.9399090570441</v>
-      </c>
-    </row>
-    <row r="111" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B111" s="7">
+      <c r="C111" s="11">
+        <v>1445.7079871938527</v>
+      </c>
+    </row>
+    <row r="112" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B112" s="7">
         <f t="shared" si="1"/>
         <v>43965</v>
       </c>
-      <c r="C111" s="11">
-        <v>1539.7720457046748</v>
-      </c>
-    </row>
-    <row r="112" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B112" s="7">
+      <c r="C112" s="11">
+        <v>1279.8674474269685</v>
+      </c>
+    </row>
+    <row r="113" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B113" s="7">
         <f t="shared" si="1"/>
         <v>43980</v>
       </c>
-      <c r="C112" s="11">
-        <v>1558.5115652939269</v>
-      </c>
-    </row>
-    <row r="113" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B113" s="7">
+      <c r="C113" s="11">
+        <v>1287.9056745528653</v>
+      </c>
+    </row>
+    <row r="114" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B114" s="7">
         <f t="shared" si="1"/>
         <v>43995</v>
       </c>
-      <c r="C113" s="11">
-        <v>1573.2632442473425</v>
-      </c>
-    </row>
-    <row r="114" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B114" s="7">
+      <c r="C114" s="11">
+        <v>1296.6593342879682</v>
+      </c>
+    </row>
+    <row r="115" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B115" s="7">
         <f t="shared" si="1"/>
         <v>44010</v>
       </c>
-      <c r="C114" s="11">
-        <v>1592.1479094859324</v>
-      </c>
-    </row>
-    <row r="115" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B115" s="7">
+      <c r="C115" s="11">
+        <v>1313.9701291870786</v>
+      </c>
+    </row>
+    <row r="116" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B116" s="7">
         <f t="shared" si="1"/>
         <v>44025</v>
       </c>
-      <c r="C115" s="11">
-        <v>1599.1224529891049</v>
-      </c>
-    </row>
-    <row r="116" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B116" s="7">
+      <c r="C116" s="11">
+        <v>1337.5356523283872</v>
+      </c>
+    </row>
+    <row r="117" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B117" s="7">
         <f t="shared" si="1"/>
         <v>44040</v>
       </c>
-      <c r="C116" s="11">
-        <v>1615.786301334294</v>
-      </c>
-    </row>
-    <row r="117" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B117" s="7">
+      <c r="C117" s="11">
+        <v>1348.3240250964293</v>
+      </c>
+    </row>
+    <row r="118" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B118" s="7">
         <f t="shared" si="1"/>
         <v>44055</v>
       </c>
-      <c r="C117" s="11">
-        <v>1411.0080210997874</v>
-      </c>
-    </row>
-    <row r="118" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B118" s="7">
+      <c r="C118" s="11">
+        <v>1162.8244231391045</v>
+      </c>
+    </row>
+    <row r="119" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B119" s="7">
         <f t="shared" si="1"/>
         <v>44070</v>
       </c>
-      <c r="C118" s="11">
-        <v>1424.2263678418358</v>
-      </c>
-    </row>
-    <row r="119" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B119" s="7">
+      <c r="C119" s="11">
+        <v>1165.2286023690199</v>
+      </c>
+    </row>
+    <row r="120" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B120" s="7">
         <f t="shared" si="1"/>
         <v>44085</v>
       </c>
-      <c r="C119" s="11">
-        <v>1435.6297353612122</v>
-      </c>
-    </row>
-    <row r="120" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B120" s="7">
+      <c r="C120" s="11">
+        <v>1166.1137329123385</v>
+      </c>
+    </row>
+    <row r="121" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B121" s="7">
         <f t="shared" si="1"/>
         <v>44100</v>
       </c>
-      <c r="C120" s="11">
-        <v>1444.5939620911495</v>
-      </c>
-    </row>
-    <row r="121" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B121" s="7">
+      <c r="C121" s="11">
+        <v>1174.9505611698819</v>
+      </c>
+    </row>
+    <row r="122" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B122" s="7">
         <f t="shared" si="1"/>
         <v>44115</v>
       </c>
-      <c r="C121" s="11">
-        <v>1454.9311122201282</v>
-      </c>
-    </row>
-    <row r="122" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B122" s="7">
+      <c r="C122" s="11">
+        <v>1187.1988058998409</v>
+      </c>
+    </row>
+    <row r="123" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B123" s="7">
         <f t="shared" si="1"/>
         <v>44130</v>
       </c>
-      <c r="C122" s="11">
-        <v>1473.7640670957662</v>
-      </c>
-    </row>
-    <row r="123" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B123" s="7">
+      <c r="C123" s="11">
+        <v>1198.7151861639536</v>
+      </c>
+    </row>
+    <row r="124" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B124" s="7">
         <f t="shared" si="1"/>
         <v>44145</v>
       </c>
-      <c r="C123" s="11">
-        <v>1243.1443655145872</v>
-      </c>
-    </row>
-    <row r="124" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B124" s="7">
+      <c r="C124" s="11">
+        <v>990.48320610803239</v>
+      </c>
+    </row>
+    <row r="125" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B125" s="7">
         <f t="shared" si="1"/>
         <v>44160</v>
       </c>
-      <c r="C124" s="11">
-        <v>1246.458772956863</v>
-      </c>
-    </row>
-    <row r="125" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B125" s="7">
+      <c r="C125" s="11">
+        <v>991.71025151818696</v>
+      </c>
+    </row>
+    <row r="126" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B126" s="7">
         <f t="shared" si="1"/>
         <v>44175</v>
       </c>
-      <c r="C125" s="11">
-        <v>1250.1801245204556</v>
-      </c>
-    </row>
-    <row r="126" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B126" s="7">
+      <c r="C126" s="11">
+        <v>1004.7614445840968</v>
+      </c>
+    </row>
+    <row r="127" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B127" s="7">
         <f t="shared" si="1"/>
         <v>44190</v>
       </c>
-      <c r="C126" s="11">
-        <v>1258.4100830775412</v>
-      </c>
-    </row>
-    <row r="127" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B127" s="7">
+      <c r="C127" s="11">
+        <v>1007.2397743879393</v>
+      </c>
+    </row>
+    <row r="128" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B128" s="7">
         <f t="shared" si="1"/>
         <v>44205</v>
       </c>
-      <c r="C127" s="11">
-        <v>1268.7283489824581</v>
-      </c>
-    </row>
-    <row r="128" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B128" s="7">
+      <c r="C128" s="11">
+        <v>1020.5489770455223</v>
+      </c>
+    </row>
+    <row r="129" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B129" s="7">
         <f t="shared" si="1"/>
         <v>44220</v>
       </c>
-      <c r="C128" s="11">
-        <v>1281.005602806465</v>
-      </c>
-    </row>
-    <row r="129" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B129" s="7">
+      <c r="C129" s="11">
+        <v>1030.2241902087057</v>
+      </c>
+    </row>
+    <row r="130" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B130" s="7">
         <f t="shared" si="1"/>
         <v>44235</v>
       </c>
-      <c r="C129" s="11">
-        <v>1029.7735675214969</v>
-      </c>
-    </row>
-    <row r="130" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B130" s="7">
+      <c r="C130" s="11">
+        <v>801.98707976094056</v>
+      </c>
+    </row>
+    <row r="131" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B131" s="7">
         <f t="shared" si="1"/>
         <v>44250</v>
       </c>
-      <c r="C130" s="11">
-        <v>1037.1564459421438</v>
-      </c>
-    </row>
-    <row r="131" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B131" s="7">
+      <c r="C131" s="11">
+        <v>804.93363602883016</v>
+      </c>
+    </row>
+    <row r="132" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B132" s="7">
         <f t="shared" si="1"/>
         <v>44265</v>
       </c>
-      <c r="C131" s="11">
-        <v>1039.5975938678268</v>
-      </c>
-    </row>
-    <row r="132" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B132" s="7">
+      <c r="C132" s="11">
+        <v>808.88846947213813</v>
+      </c>
+    </row>
+    <row r="133" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B133" s="7">
         <f t="shared" si="1"/>
         <v>44280</v>
       </c>
-      <c r="C132" s="11">
-        <v>1045.1321244180285</v>
-      </c>
-    </row>
-    <row r="133" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B133" s="7">
+      <c r="C133" s="11">
+        <v>814.11579808135559</v>
+      </c>
+    </row>
+    <row r="134" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B134" s="7">
         <f t="shared" si="1"/>
         <v>44295</v>
       </c>
-      <c r="C133" s="11">
-        <v>1048.2314218646941</v>
-      </c>
-    </row>
-    <row r="134" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B134" s="7">
+      <c r="C134" s="11">
+        <v>822.31900902957466</v>
+      </c>
+    </row>
+    <row r="135" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B135" s="7">
         <f t="shared" si="1"/>
         <v>44310</v>
       </c>
-      <c r="C134" s="11">
-        <v>1059.2601865500501</v>
-      </c>
-    </row>
-    <row r="135" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B135" s="7">
+      <c r="C135" s="11">
+        <v>823.41895797462337</v>
+      </c>
+    </row>
+    <row r="136" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B136" s="7">
         <f t="shared" si="1"/>
         <v>44325</v>
       </c>
-      <c r="C135" s="11">
-        <v>784.38358582574813</v>
-      </c>
-    </row>
-    <row r="136" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B136" s="7">
+      <c r="C136" s="11">
+        <v>577.98199238304335</v>
+      </c>
+    </row>
+    <row r="137" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B137" s="7">
         <f t="shared" si="1"/>
         <v>44340</v>
       </c>
-      <c r="C136" s="11">
-        <v>784.51568238942559</v>
-      </c>
-    </row>
-    <row r="137" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B137" s="7">
+      <c r="C137" s="11">
+        <v>577.89956794405691</v>
+      </c>
+    </row>
+    <row r="138" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B138" s="7">
         <f t="shared" si="1"/>
         <v>44355</v>
       </c>
-      <c r="C137" s="11">
-        <v>784.59397650783626</v>
-      </c>
-    </row>
-    <row r="138" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B138" s="7">
+      <c r="C138" s="11">
+        <v>578.26982912862229</v>
+      </c>
+    </row>
+    <row r="139" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B139" s="7">
         <f t="shared" si="1"/>
         <v>44370</v>
       </c>
-      <c r="C138" s="11">
-        <v>785.95759562746662</v>
-      </c>
-    </row>
-    <row r="139" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B139" s="7">
+      <c r="C139" s="11">
+        <v>578.57441240430626</v>
+      </c>
+    </row>
+    <row r="140" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B140" s="7">
         <f t="shared" si="1"/>
         <v>44385</v>
       </c>
-      <c r="C139" s="11">
-        <v>787.44073155746662</v>
-      </c>
-    </row>
-    <row r="140" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B140" s="7">
+      <c r="C140" s="11">
+        <v>578.92070392709491</v>
+      </c>
+    </row>
+    <row r="141" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B141" s="7">
         <f t="shared" si="1"/>
         <v>44400</v>
       </c>
-      <c r="C140" s="11">
-        <v>789.2823395128255</v>
-      </c>
-    </row>
-    <row r="141" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B141" s="7">
+      <c r="C141" s="11">
+        <v>578.84052317282317</v>
+      </c>
+    </row>
+    <row r="142" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B142" s="7">
         <f t="shared" si="1"/>
         <v>44415</v>
       </c>
-      <c r="C141" s="11">
-        <v>485.32972976694367</v>
-      </c>
-    </row>
-    <row r="142" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B142" s="7">
+      <c r="C142" s="11">
+        <v>306.59207131272933</v>
+      </c>
+    </row>
+    <row r="143" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B143" s="7">
         <f t="shared" si="1"/>
         <v>44430</v>
       </c>
-      <c r="C142" s="11">
-        <v>479.95788106267059</v>
-      </c>
-    </row>
-    <row r="143" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B143" s="7">
+      <c r="C143" s="11">
+        <v>303.14322533324707</v>
+      </c>
+    </row>
+    <row r="144" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B144" s="7">
         <f t="shared" si="1"/>
         <v>44445</v>
       </c>
-      <c r="C143" s="11">
-        <v>473.81021110626386</v>
-      </c>
-    </row>
-    <row r="144" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B144" s="7">
+      <c r="C144" s="11">
+        <v>299.3380272572042</v>
+      </c>
+    </row>
+    <row r="145" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B145" s="7">
         <f t="shared" si="1"/>
         <v>44460</v>
       </c>
-      <c r="C144" s="11">
-        <v>469.43690998874439</v>
-      </c>
-    </row>
-    <row r="145" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B145" s="7">
+      <c r="C145" s="11">
+        <v>293.79157339572407</v>
+      </c>
+    </row>
+    <row r="146" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B146" s="7">
         <f t="shared" si="1"/>
         <v>44475</v>
       </c>
-      <c r="C145" s="11">
-        <v>464.80849303355564</v>
-      </c>
-    </row>
-    <row r="146" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B146" s="7">
+      <c r="C146" s="11">
+        <v>289.7923352371858</v>
+      </c>
+    </row>
+    <row r="147" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B147" s="7">
         <f t="shared" si="1"/>
         <v>44490</v>
       </c>
-      <c r="C146" s="11">
-        <v>459.815138814985</v>
+      <c r="C147" s="11">
+        <v>285.63079090851278</v>
       </c>
     </row>
   </sheetData>
@@ -2876,18 +2917,18 @@
   <dimension ref="B2:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="B6" sqref="B6:C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="35.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.88671875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:7" ht="15" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
@@ -2901,7 +2942,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:7" ht="15" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
@@ -2915,7 +2956,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:7" ht="15" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>3</v>
       </c>
@@ -2923,13 +2964,13 @@
         <v>8.9999999999999993E-3</v>
       </c>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:7" ht="15" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="6" t="str">
         <f>G9</f>
-        <v>ZARSwap.09:10:26-123</v>
+        <v>ZARSwap.21:15:14-6</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>9</v>
@@ -2938,12 +2979,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:7" ht="15" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>12</v>
+        <v>35</v>
       </c>
       <c r="F6" s="7">
         <v>42675</v>
@@ -2952,7 +2993,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:7" ht="15" x14ac:dyDescent="0.25">
       <c r="F7" s="7">
         <v>46327</v>
       </c>
@@ -2965,14 +3006,14 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:7" ht="15" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="str">
         <f>_xll.QSA.CreateHWModelDemo(C2,C3,C4,C5,C6)</f>
-        <v>HWDemo.09:10:26-124</v>
+        <v>HWDemo.21:15:14-7</v>
       </c>
       <c r="G9" s="3" t="str">
         <f>_xll.QSA.CreateDatesAndRatesCurve(G2,F6:F7,G6:G7,G3)</f>
-        <v>ZARSwap.09:10:26-123</v>
+        <v>ZARSwap.21:15:14-6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>